<commit_message>
small updates for running code
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD0BE2B-7664-DA4C-A463-4BBF6E46C87E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EDCFB1-7C5C-4049-91D4-C9C75696088A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="-20720" windowWidth="21560" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="68">
   <si>
     <t>country</t>
   </si>
@@ -204,6 +204,42 @@
   </si>
   <si>
     <t>20-030971_G2_Main_Wave3_Merged_FI LI CH_v1_16032021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave6_Final_v1_26032021_IntClientUse</t>
+  </si>
+  <si>
+    <t>at_sr07_20210325_pA_wv06</t>
+  </si>
+  <si>
+    <t>dk_sr07_20210325_pA_wv06</t>
+  </si>
+  <si>
+    <t>fr_sr07_20210325_pA_wv06</t>
+  </si>
+  <si>
+    <t>it_sr07_20210325_pA_wv06</t>
+  </si>
+  <si>
+    <t>pl_sr07_20210325_pA_wv06</t>
+  </si>
+  <si>
+    <t>es_sr06_20210325_pA_wv06</t>
+  </si>
+  <si>
+    <t>pt_sr06_19000100_pA_wv06</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave4_Merged_FI LI CH_v1_29032021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave2_Merged_SL EL_v1_29032021_IntClientUse</t>
+  </si>
+  <si>
+    <t>Greece is 2 survey round behind other G2 countries (1 round was unusable)</t>
+  </si>
+  <si>
+    <t>download</t>
   </si>
 </sst>
 </file>
@@ -601,1250 +637,1583 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
-        <v>4</v>
+      <c r="B2" s="2">
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>44207</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="str">
-        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+      <c r="J2" t="str">
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3">
-        <v>4</v>
+      <c r="B3" s="2">
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>44207</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I41" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+      <c r="J3" s="2" t="str">
+        <f t="shared" ref="J3:J41" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4">
-        <v>4</v>
+      <c r="B4" s="2">
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
         <v>44207</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="B5" s="2">
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
         <v>44207</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6">
-        <v>4</v>
+      <c r="B6" s="2">
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
         <v>44207</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
         <v>44207</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
         <v>44207</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="2" t="str">
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pt_sr01_20210118_pA_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>44214</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="2" t="str">
+      <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>44214</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11">
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
         <v>2</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>44214</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>44214</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="2" t="str">
+      <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13">
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13">
         <v>2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>44214</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="2" t="str">
+      <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14">
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14">
         <v>2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>44214</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="2" t="str">
+      <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="2">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
       </c>
       <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15">
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>44214</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="2" t="str">
+      <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pt_sr02_20210129_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2">
         <v>3</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>44225</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="2" t="str">
+      <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>44225</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="2" t="str">
+      <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
         <v>3</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2">
         <v>3</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>44225</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="2" t="str">
+      <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="2">
         <v>3</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>44225</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="2" t="str">
+      <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
         <v>3</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="2">
         <v>3</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>44225</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="2" t="str">
+      <c r="J20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
         <v>3</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2">
         <v>3</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>44225</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="2" t="str">
+      <c r="J21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
         <v>3</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2">
         <v>3</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>44225</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="2" t="str">
+      <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pt_sr03_20210111_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2">
-        <v>4</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
       </c>
       <c r="D23" s="4">
-        <v>4</v>
-      </c>
-      <c r="E23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="4">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
         <v>44207</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="2" t="str">
+      <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="2">
-        <v>4</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4</v>
       </c>
       <c r="D24" s="4">
-        <v>4</v>
-      </c>
-      <c r="E24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>4</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
         <v>44207</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I24" s="2" t="str">
+      <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="2">
-        <v>4</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4</v>
       </c>
       <c r="D25" s="4">
-        <v>4</v>
-      </c>
-      <c r="E25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
         <v>44207</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="2" t="str">
+      <c r="J25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="2">
-        <v>4</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4</v>
       </c>
       <c r="D26" s="4">
-        <v>4</v>
-      </c>
-      <c r="E26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
         <v>44207</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I26" s="2" t="str">
+      <c r="J26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="4">
-        <v>4</v>
+      <c r="B27" s="2">
+        <v>1</v>
       </c>
       <c r="C27" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D27" s="4">
-        <v>4</v>
-      </c>
-      <c r="E27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
         <v>44207</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="2" t="str">
+      <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr04_20210226_pC_wv01</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B28">
-        <v>4</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
         <v>5</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="4">
-        <v>4</v>
-      </c>
-      <c r="G28" s="3">
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="4">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3">
         <v>44253</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>49</v>
       </c>
-      <c r="I28" s="2" t="str">
+      <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
         <v>5</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="4">
-        <v>4</v>
-      </c>
-      <c r="G29" s="3">
+      <c r="F29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="4">
+        <v>4</v>
+      </c>
+      <c r="H29" s="3">
         <v>44253</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I29" s="2" t="str">
+      <c r="J29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-      <c r="C30" s="4">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
         <v>5</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="4">
-        <v>4</v>
-      </c>
-      <c r="G30" s="3">
+      <c r="F30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="4">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3">
         <v>44253</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I30" s="2" t="str">
+      <c r="J30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
         <v>5</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="4">
-        <v>4</v>
-      </c>
-      <c r="G31" s="3">
+      <c r="F31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="4">
+        <v>4</v>
+      </c>
+      <c r="H31" s="3">
         <v>44253</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I31" s="2" t="str">
+      <c r="J31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0</v>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
       </c>
       <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
         <v>5</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="4">
-        <v>4</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="F32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="4">
+        <v>4</v>
+      </c>
+      <c r="H32" s="3">
         <v>44253</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="2" t="str">
+      <c r="J32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
       </c>
       <c r="D33" s="2">
-        <v>4</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="4">
-        <v>4</v>
-      </c>
-      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4</v>
+      </c>
+      <c r="H33" s="3">
         <v>44253</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I33" s="2" t="str">
+      <c r="J33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr04_20210226_pA_wv04</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
       </c>
       <c r="D34" s="2">
-        <v>4</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="4">
-        <v>4</v>
-      </c>
-      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="4">
+        <v>4</v>
+      </c>
+      <c r="H34" s="3">
         <v>44253</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I34" s="2" t="str">
+      <c r="J34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pt_sr04_20210316_pA_wv04</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="D35">
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="E35">
         <v>6</v>
       </c>
-      <c r="E35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="4">
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="4">
         <v>5</v>
       </c>
-      <c r="G35" s="3">
+      <c r="H35" s="3">
         <v>44271</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>53</v>
       </c>
-      <c r="I35" s="2" t="str">
+      <c r="J35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="2">
-        <v>4</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2">
         <v>6</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="4">
+      <c r="F36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="4">
         <v>5</v>
       </c>
-      <c r="G36" s="3">
+      <c r="H36" s="3">
         <v>44271</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I36" s="2" t="str">
+      <c r="J36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="2">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2">
         <v>6</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="4">
+      <c r="F37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="4">
         <v>5</v>
       </c>
-      <c r="G37" s="3">
+      <c r="H37" s="3">
         <v>44271</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I37" s="2" t="str">
+      <c r="J37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B38" s="2">
-        <v>4</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2">
         <v>6</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="4">
+      <c r="F38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="4">
         <v>5</v>
       </c>
-      <c r="G38" s="3">
+      <c r="H38" s="3">
         <v>44271</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I38" s="2" t="str">
+      <c r="J38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B39" s="2">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2">
         <v>6</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="4">
+      <c r="F39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="4">
         <v>5</v>
       </c>
-      <c r="G39" s="3">
+      <c r="H39" s="3">
         <v>44271</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="2" t="str">
+      <c r="J39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="2">
-        <v>4</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2">
         <v>5</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="4">
+      <c r="F40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="4">
         <v>5</v>
       </c>
-      <c r="G40" s="3">
+      <c r="H40" s="3">
         <v>44271</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I40" s="2" t="str">
+      <c r="J40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="4">
-        <v>4</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4">
+        <v>4</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4">
         <v>5</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="4">
+      <c r="F41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="4">
         <v>5</v>
       </c>
-      <c r="G41" s="5">
+      <c r="H41" s="5">
         <v>44271</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>pt_sr05_19000100_pA_wv05</v>
+      <c r="J41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr05_20210325_pA_wv05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I42" t="s">
+        <v>56</v>
+      </c>
+      <c r="J42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I43" t="s">
+        <v>56</v>
+      </c>
+      <c r="J43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44">
+        <v>6</v>
+      </c>
+      <c r="H44" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I44" t="s">
+        <v>56</v>
+      </c>
+      <c r="J44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>6</v>
+      </c>
+      <c r="H45" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I45" t="s">
+        <v>56</v>
+      </c>
+      <c r="J45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>6</v>
+      </c>
+      <c r="H46" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I46" t="s">
+        <v>56</v>
+      </c>
+      <c r="J46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="H47" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I47" t="s">
+        <v>56</v>
+      </c>
+      <c r="J47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>6</v>
+      </c>
+      <c r="F48" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48">
+        <v>6</v>
+      </c>
+      <c r="H48" s="3">
+        <v>44280</v>
+      </c>
+      <c r="I48" t="s">
+        <v>56</v>
+      </c>
+      <c r="J48" t="s">
+        <v>63</v>
+      </c>
+      <c r="K48" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1854,517 +2223,719 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.1640625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.1640625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
         <v>44207</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="2" t="str">
-        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+      <c r="J2" s="2" t="str">
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
         <v>lt_sr01_20210112_pA_wv01</v>
       </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
         <v>44208</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I16" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+      <c r="J3" s="2" t="str">
+        <f t="shared" ref="J3:J21" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>fi_sr01_20210113_pA_wv01</v>
       </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
         <v>44209</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr01_20210112_pA_wv01</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4</v>
       </c>
       <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
         <v>44208</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fi_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="4">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
       </c>
       <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
         <v>44209</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
         <v>44209</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>gr_sr01_20210111_pC_wv01</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
       </c>
       <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
         <v>44207</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="2" t="str">
+      <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>lt_sr02_20210304_pC_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>3</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>44259</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="2" t="str">
+      <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>lt_sr03_20210305_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>44260</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fi_sr03_20210306_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11">
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
         <v>2</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>44261</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr03_20210307_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12">
-        <v>4</v>
+      <c r="B12" s="2">
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
         <v>44262</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="2" t="str">
+      <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>gr_sr02_20210316_pA_wv01</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
         <v>44271</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="2" t="str">
+      <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>si_sr01_20210316_pA_wv01</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="4">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>44271</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="2" t="str">
+      <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fi_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="4">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2">
-        <v>4</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2">
         <v>3</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>44271</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="2" t="str">
+      <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2">
-        <v>4</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2">
         <v>3</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>44271</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>lt_sr04_19000100_pA_wv03</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="2"/>
+      <c r="J16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr04_20210329_pA_wv03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3">
+        <v>44284</v>
+      </c>
+      <c r="I17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr05_20210329_pA_wv04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" s="3">
+        <v>44284</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr05_20210329_pA_wv04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" s="3">
+        <v>44284</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr05_20210329_pA_wv04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>44284</v>
+      </c>
+      <c r="I20" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>si_sr02_20210329_pA_wv02</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>44284</v>
+      </c>
+      <c r="I21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>gr_sr03_19000100_pA_wv02</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
child data g1 13-4
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EDCFB1-7C5C-4049-91D4-C9C75696088A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6EF276-6C85-2A43-BFAF-E83EFF866AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="-20720" windowWidth="21560" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="-20720" windowWidth="21560" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="64">
   <si>
     <t>country</t>
   </si>
@@ -209,27 +209,6 @@
     <t>20-030971_G1_Merged_Wave6_Final_v1_26032021_IntClientUse</t>
   </si>
   <si>
-    <t>at_sr07_20210325_pA_wv06</t>
-  </si>
-  <si>
-    <t>dk_sr07_20210325_pA_wv06</t>
-  </si>
-  <si>
-    <t>fr_sr07_20210325_pA_wv06</t>
-  </si>
-  <si>
-    <t>it_sr07_20210325_pA_wv06</t>
-  </si>
-  <si>
-    <t>pl_sr07_20210325_pA_wv06</t>
-  </si>
-  <si>
-    <t>es_sr06_20210325_pA_wv06</t>
-  </si>
-  <si>
-    <t>pt_sr06_19000100_pA_wv06</t>
-  </si>
-  <si>
     <t>20-030971_G2_Main_Wave4_Merged_FI LI CH_v1_29032021_IntClientUse</t>
   </si>
   <si>
@@ -240,13 +219,22 @@
   </si>
   <si>
     <t>download</t>
+  </si>
+  <si>
+    <t>20-030971-01_G1_PT&amp;ES_Wave1_Parents_Final_v1_13042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_01_G1_Merged_Wave2_Parents_Final_v1_13042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>ES &amp; PT 1 round behind (1 children's round)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +245,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,13 +284,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -657,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -700,9 +703,6 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
       <c r="C2">
         <v>4</v>
       </c>
@@ -733,9 +733,6 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
       <c r="C3">
         <v>4</v>
       </c>
@@ -758,7 +755,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J41" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <f t="shared" ref="J3:J55" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
@@ -766,9 +763,6 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
       <c r="C4">
         <v>4</v>
       </c>
@@ -799,9 +793,6 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
       <c r="C5">
         <v>4</v>
       </c>
@@ -832,9 +823,6 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
       <c r="C6">
         <v>4</v>
       </c>
@@ -865,9 +853,6 @@
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
       <c r="C7" s="2">
         <v>4</v>
       </c>
@@ -898,9 +883,6 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
@@ -931,9 +913,6 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
       <c r="C9" s="2">
         <v>4</v>
       </c>
@@ -964,9 +943,6 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
       <c r="C10" s="2">
         <v>4</v>
       </c>
@@ -997,9 +973,6 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
       <c r="C11" s="2">
         <v>4</v>
       </c>
@@ -1030,9 +1003,6 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
       <c r="C12" s="2">
         <v>4</v>
       </c>
@@ -1063,9 +1033,6 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
@@ -1096,9 +1063,6 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
       <c r="C14" s="2">
         <v>4</v>
       </c>
@@ -1129,9 +1093,6 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
       <c r="C15" s="2">
         <v>4</v>
       </c>
@@ -1162,9 +1123,6 @@
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
       <c r="C16" s="2">
         <v>4</v>
       </c>
@@ -1195,9 +1153,6 @@
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
       <c r="C17" s="2">
         <v>4</v>
       </c>
@@ -1228,9 +1183,6 @@
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
       <c r="C18" s="2">
         <v>4</v>
       </c>
@@ -1261,9 +1213,6 @@
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
       <c r="C19" s="2">
         <v>4</v>
       </c>
@@ -1294,9 +1243,6 @@
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
       <c r="C20" s="2">
         <v>4</v>
       </c>
@@ -1327,9 +1273,6 @@
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
       <c r="C21" s="2">
         <v>4</v>
       </c>
@@ -1360,9 +1303,6 @@
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
       <c r="C22" s="2">
         <v>4</v>
       </c>
@@ -1393,9 +1333,6 @@
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
       <c r="C23" s="2">
         <v>4</v>
       </c>
@@ -1426,9 +1363,6 @@
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
       <c r="C24" s="2">
         <v>4</v>
       </c>
@@ -1459,9 +1393,6 @@
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
       <c r="C25" s="2">
         <v>4</v>
       </c>
@@ -1492,9 +1423,6 @@
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="2">
-        <v>1</v>
-      </c>
       <c r="C26" s="2">
         <v>4</v>
       </c>
@@ -1525,9 +1453,6 @@
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
@@ -1558,9 +1483,6 @@
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
       <c r="C28">
         <v>4</v>
       </c>
@@ -1591,9 +1513,6 @@
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
       <c r="C29">
         <v>4</v>
       </c>
@@ -1624,9 +1543,6 @@
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="2">
-        <v>1</v>
-      </c>
       <c r="C30">
         <v>4</v>
       </c>
@@ -1657,9 +1573,6 @@
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
       <c r="C31">
         <v>4</v>
       </c>
@@ -1690,9 +1603,6 @@
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
       <c r="C32">
         <v>4</v>
       </c>
@@ -1723,9 +1633,6 @@
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="2">
-        <v>1</v>
-      </c>
       <c r="C33">
         <v>4</v>
       </c>
@@ -1759,9 +1666,6 @@
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
       <c r="C34">
         <v>4</v>
       </c>
@@ -1795,9 +1699,6 @@
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
       <c r="C35">
         <v>4</v>
       </c>
@@ -1825,9 +1726,6 @@
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="2">
-        <v>1</v>
-      </c>
       <c r="C36" s="2">
         <v>4</v>
       </c>
@@ -1856,9 +1754,6 @@
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
       <c r="C37" s="2">
         <v>4</v>
       </c>
@@ -1887,9 +1782,6 @@
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="2">
-        <v>1</v>
-      </c>
       <c r="C38" s="2">
         <v>4</v>
       </c>
@@ -1918,9 +1810,6 @@
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="2">
-        <v>1</v>
-      </c>
       <c r="C39" s="2">
         <v>4</v>
       </c>
@@ -1949,9 +1838,6 @@
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="2">
-        <v>1</v>
-      </c>
       <c r="C40" s="2">
         <v>4</v>
       </c>
@@ -1980,9 +1866,6 @@
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="2">
-        <v>1</v>
-      </c>
       <c r="C41" s="4">
         <v>4</v>
       </c>
@@ -2011,9 +1894,6 @@
       <c r="A42" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
       <c r="C42">
         <v>4</v>
       </c>
@@ -2032,17 +1912,15 @@
       <c r="I42" t="s">
         <v>56</v>
       </c>
-      <c r="J42" t="s">
-        <v>57</v>
+      <c r="J42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>at_sr07_20210325_pA_wv06</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
       <c r="C43">
         <v>4</v>
       </c>
@@ -2061,17 +1939,15 @@
       <c r="I43" t="s">
         <v>56</v>
       </c>
-      <c r="J43" t="s">
-        <v>58</v>
+      <c r="J43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_sr07_20210325_pA_wv06</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="2">
-        <v>1</v>
-      </c>
       <c r="C44">
         <v>4</v>
       </c>
@@ -2090,17 +1966,15 @@
       <c r="I44" t="s">
         <v>56</v>
       </c>
-      <c r="J44" t="s">
-        <v>59</v>
+      <c r="J44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr07_20210325_pA_wv06</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
       <c r="C45">
         <v>4</v>
       </c>
@@ -2119,17 +1993,15 @@
       <c r="I45" t="s">
         <v>56</v>
       </c>
-      <c r="J45" t="s">
-        <v>60</v>
+      <c r="J45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr07_20210325_pA_wv06</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
       <c r="C46">
         <v>4</v>
       </c>
@@ -2148,12 +2020,13 @@
       <c r="I46" t="s">
         <v>56</v>
       </c>
-      <c r="J46" t="s">
-        <v>61</v>
+      <c r="J46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr07_20210325_pA_wv06</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="2">
@@ -2177,15 +2050,16 @@
       <c r="I47" t="s">
         <v>56</v>
       </c>
-      <c r="J47" t="s">
-        <v>62</v>
+      <c r="J47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr06_20210325_pA_wv06</v>
       </c>
       <c r="K47" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="2">
@@ -2209,14 +2083,211 @@
       <c r="I48" t="s">
         <v>56</v>
       </c>
-      <c r="J48" t="s">
-        <v>63</v>
+      <c r="J48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr06_20210413_pA_wv06</v>
       </c>
       <c r="K48" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="6">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr07_20210413_pC_wv01</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr07_20210413_pC_wv01</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I51" t="s">
+        <v>62</v>
+      </c>
+      <c r="J51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>at_sr08_20210413_pC_wv02</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_sr08_20210413_pC_wv02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="2">
+        <v>2</v>
+      </c>
+      <c r="H53" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr08_20210413_pC_wv02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2</v>
+      </c>
+      <c r="H54" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr08_20210413_pC_wv02</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="2">
+        <v>2</v>
+      </c>
+      <c r="H55" s="3">
+        <v>44299</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr08_19000100_pC_wv02</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2225,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2249,7 +2320,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>12</v>
@@ -2804,7 +2875,7 @@
         <v>44284</v>
       </c>
       <c r="I17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2834,7 +2905,7 @@
         <v>44284</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2864,7 +2935,7 @@
         <v>44284</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2894,14 +2965,14 @@
         <v>44284</v>
       </c>
       <c r="I20" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>si_sr02_20210329_pA_wv02</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2927,7 +2998,7 @@
         <v>44284</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
set to download all
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6EF276-6C85-2A43-BFAF-E83EFF866AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF9612-A506-9243-AFBA-AE4A91DE7BC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="-20720" windowWidth="21560" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="-20720" windowWidth="21560" windowHeight="20520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -703,6 +703,9 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
       <c r="C2">
         <v>4</v>
       </c>
@@ -733,6 +736,9 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
       <c r="C3">
         <v>4</v>
       </c>
@@ -763,6 +769,9 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
       <c r="C4">
         <v>4</v>
       </c>
@@ -793,6 +802,9 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
       <c r="C5">
         <v>4</v>
       </c>
@@ -823,6 +835,9 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
       <c r="C6">
         <v>4</v>
       </c>
@@ -853,6 +868,9 @@
       <c r="A7" t="s">
         <v>24</v>
       </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="2">
         <v>4</v>
       </c>
@@ -883,6 +901,9 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
@@ -913,6 +934,9 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
       <c r="C9" s="2">
         <v>4</v>
       </c>
@@ -943,6 +967,9 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
       <c r="C10" s="2">
         <v>4</v>
       </c>
@@ -973,6 +1000,9 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
       <c r="C11" s="2">
         <v>4</v>
       </c>
@@ -1003,6 +1033,9 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
       <c r="C12" s="2">
         <v>4</v>
       </c>
@@ -1033,6 +1066,9 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
@@ -1063,6 +1099,9 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
       <c r="C14" s="2">
         <v>4</v>
       </c>
@@ -1093,6 +1132,9 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
       <c r="C15" s="2">
         <v>4</v>
       </c>
@@ -1123,6 +1165,9 @@
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
       <c r="C16" s="2">
         <v>4</v>
       </c>
@@ -1153,6 +1198,9 @@
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
       <c r="C17" s="2">
         <v>4</v>
       </c>
@@ -1183,6 +1231,9 @@
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
       <c r="C18" s="2">
         <v>4</v>
       </c>
@@ -1213,6 +1264,9 @@
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
       <c r="C19" s="2">
         <v>4</v>
       </c>
@@ -1243,6 +1297,9 @@
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
       <c r="C20" s="2">
         <v>4</v>
       </c>
@@ -1273,6 +1330,9 @@
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
       <c r="C21" s="2">
         <v>4</v>
       </c>
@@ -1303,6 +1363,9 @@
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
       <c r="C22" s="2">
         <v>4</v>
       </c>
@@ -1333,6 +1396,9 @@
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
       <c r="C23" s="2">
         <v>4</v>
       </c>
@@ -1363,6 +1429,9 @@
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
       <c r="C24" s="2">
         <v>4</v>
       </c>
@@ -1393,6 +1462,9 @@
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
       <c r="C25" s="2">
         <v>4</v>
       </c>
@@ -1423,6 +1495,9 @@
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
       <c r="C26" s="2">
         <v>4</v>
       </c>
@@ -1453,6 +1528,9 @@
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
@@ -1483,6 +1561,9 @@
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
       <c r="C28">
         <v>4</v>
       </c>
@@ -1513,6 +1594,9 @@
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
       <c r="C29">
         <v>4</v>
       </c>
@@ -1543,6 +1627,9 @@
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
       <c r="C30">
         <v>4</v>
       </c>
@@ -1573,6 +1660,9 @@
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
       <c r="C31">
         <v>4</v>
       </c>
@@ -1603,6 +1693,9 @@
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
       <c r="C32">
         <v>4</v>
       </c>
@@ -1633,6 +1726,9 @@
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
       <c r="C33">
         <v>4</v>
       </c>
@@ -1666,6 +1762,9 @@
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
       <c r="C34">
         <v>4</v>
       </c>
@@ -1699,6 +1798,9 @@
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
       <c r="C35">
         <v>4</v>
       </c>
@@ -1726,6 +1828,9 @@
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
       <c r="C36" s="2">
         <v>4</v>
       </c>
@@ -1754,6 +1859,9 @@
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
       <c r="C37" s="2">
         <v>4</v>
       </c>
@@ -1782,6 +1890,9 @@
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
       <c r="C38" s="2">
         <v>4</v>
       </c>
@@ -1810,6 +1921,9 @@
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
       <c r="C39" s="2">
         <v>4</v>
       </c>
@@ -1838,6 +1952,9 @@
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
       <c r="C40" s="2">
         <v>4</v>
       </c>
@@ -1866,6 +1983,9 @@
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
       <c r="C41" s="4">
         <v>4</v>
       </c>
@@ -1894,6 +2014,9 @@
       <c r="A42" t="s">
         <v>19</v>
       </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
       <c r="C42">
         <v>4</v>
       </c>
@@ -1921,6 +2044,9 @@
       <c r="A43" t="s">
         <v>20</v>
       </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
       <c r="C43">
         <v>4</v>
       </c>
@@ -1948,6 +2074,9 @@
       <c r="A44" t="s">
         <v>22</v>
       </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
       <c r="C44">
         <v>4</v>
       </c>
@@ -1975,6 +2104,9 @@
       <c r="A45" t="s">
         <v>23</v>
       </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
       <c r="C45">
         <v>4</v>
       </c>
@@ -2002,6 +2134,9 @@
       <c r="A46" t="s">
         <v>24</v>
       </c>
+      <c r="B46" s="2">
+        <v>1</v>
+      </c>
       <c r="C46">
         <v>4</v>
       </c>
@@ -2095,6 +2230,9 @@
       <c r="A49" t="s">
         <v>21</v>
       </c>
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
       <c r="C49" s="6">
         <v>4</v>
       </c>
@@ -2125,6 +2263,9 @@
       <c r="A50" t="s">
         <v>25</v>
       </c>
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
       <c r="C50">
         <v>4</v>
       </c>
@@ -2155,6 +2296,9 @@
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
       <c r="C51">
         <v>4</v>
       </c>
@@ -2182,6 +2326,9 @@
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
       <c r="C52">
         <v>4</v>
       </c>
@@ -2209,6 +2356,9 @@
       <c r="A53" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
       <c r="C53">
         <v>4</v>
       </c>
@@ -2236,6 +2386,9 @@
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
       <c r="C54">
         <v>4</v>
       </c>
@@ -2262,6 +2415,9 @@
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1</v>
       </c>
       <c r="C55">
         <v>4</v>
@@ -2296,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update save country data
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805ADDC0-75AD-2345-8285-818FD23D8A37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D4859D-5F30-0549-8025-A2C10057D761}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="500" windowWidth="21560" windowHeight="16380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="24040" windowHeight="16380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -233,10 +233,10 @@
     <t>20-030971_G2_Merged_Wave2_Parents_FI LI CH EL_Final_v1_14042021_IntClientUse</t>
   </si>
   <si>
-    <t>20-030971_G2_Merged_Wave2_Parents_SL_Final_v1_14042021_IntClientUse</t>
-  </si>
-  <si>
     <t>20-030971_G2_Main_Wave3_Merged_SL EL_v1_14042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Merged_Wave1_Parents_SL_Final_v1_14042021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -2462,7 +2462,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3117,9 +3117,6 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
       <c r="C22" s="4">
         <v>4</v>
       </c>
@@ -3147,9 +3144,6 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
       <c r="C23" s="4">
         <v>4</v>
       </c>
@@ -3177,9 +3171,6 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
       <c r="C24" s="4">
         <v>4</v>
       </c>
@@ -3207,9 +3198,6 @@
       <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
       <c r="C25" s="4">
         <v>4</v>
       </c>
@@ -3253,17 +3241,17 @@
         <v>10</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="3">
         <v>44301</v>
       </c>
       <c r="I26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>si_sr03_20210415_pC_wv02</v>
+        <v>si_sr03_20210415_pC_wv01</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>52</v>
@@ -3273,9 +3261,6 @@
       <c r="A27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
@@ -3292,7 +3277,7 @@
         <v>44301</v>
       </c>
       <c r="I27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3306,9 +3291,6 @@
       <c r="A28" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
       <c r="C28" s="4">
         <v>4</v>
       </c>
@@ -3325,7 +3307,7 @@
         <v>44301</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
set all eu files to download
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D4859D-5F30-0549-8025-A2C10057D761}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F260D-F181-F241-BACF-3D3404061CEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="24040" windowHeight="16380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="24040" windowHeight="16380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
     <sheet name="G1" sheetId="6" r:id="rId2"/>
     <sheet name="G2" sheetId="8" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$28</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -651,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2461,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2522,6 +2525,9 @@
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
       <c r="C2" s="2">
         <v>4</v>
       </c>
@@ -2553,6 +2559,9 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
       <c r="C3" s="2">
         <v>4</v>
       </c>
@@ -2584,6 +2593,9 @@
       <c r="A4" t="s">
         <v>37</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
       <c r="C4" s="2">
         <v>4</v>
       </c>
@@ -2615,6 +2627,9 @@
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
       <c r="C5" s="4">
         <v>4</v>
       </c>
@@ -2645,6 +2660,9 @@
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
       <c r="C6" s="4">
         <v>4</v>
       </c>
@@ -2675,6 +2693,9 @@
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="4">
         <v>4</v>
       </c>
@@ -2708,6 +2729,9 @@
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
       <c r="C8" s="4">
         <v>4</v>
       </c>
@@ -2738,6 +2762,9 @@
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
       <c r="C9" s="2">
         <v>4</v>
       </c>
@@ -2768,6 +2795,9 @@
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
       <c r="C10" s="2">
         <v>4</v>
       </c>
@@ -2798,6 +2828,9 @@
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
       <c r="C11" s="2">
         <v>4</v>
       </c>
@@ -2828,6 +2861,9 @@
       <c r="A12" t="s">
         <v>40</v>
       </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
       <c r="C12">
         <v>4</v>
       </c>
@@ -2861,6 +2897,9 @@
       <c r="A13" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
@@ -2892,6 +2931,9 @@
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
       <c r="C14" s="4">
         <v>4</v>
       </c>
@@ -2920,6 +2962,9 @@
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
       <c r="C15" s="4">
         <v>4</v>
       </c>
@@ -2948,6 +2993,9 @@
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
       <c r="C16" s="4">
         <v>4</v>
       </c>
@@ -2976,6 +3024,9 @@
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
       <c r="C17" s="4">
         <v>4</v>
       </c>
@@ -3003,6 +3054,9 @@
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
       <c r="C18" s="4">
         <v>4</v>
       </c>
@@ -3030,6 +3084,9 @@
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
       <c r="C19" s="4">
         <v>4</v>
       </c>
@@ -3057,6 +3114,9 @@
       <c r="A20" t="s">
         <v>54</v>
       </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
       <c r="C20" s="4">
         <v>4</v>
       </c>
@@ -3087,6 +3147,9 @@
       <c r="A21" t="s">
         <v>40</v>
       </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
       <c r="C21" s="4">
         <v>4</v>
       </c>
@@ -3117,6 +3180,9 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
       <c r="C22" s="4">
         <v>4</v>
       </c>
@@ -3144,6 +3210,9 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
       <c r="C23" s="4">
         <v>4</v>
       </c>
@@ -3171,6 +3240,9 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
       <c r="C24" s="4">
         <v>4</v>
       </c>
@@ -3198,6 +3270,9 @@
       <c r="A25" t="s">
         <v>40</v>
       </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
       <c r="C25" s="4">
         <v>4</v>
       </c>
@@ -3261,6 +3336,9 @@
       <c r="A27" t="s">
         <v>40</v>
       </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
       <c r="C27" s="4">
         <v>4</v>
       </c>
@@ -3291,6 +3369,9 @@
       <c r="A28" t="s">
         <v>54</v>
       </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
       <c r="C28" s="4">
         <v>4</v>
       </c>
@@ -3318,6 +3399,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L28" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new g1 and g2 data
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414F260D-F181-F241-BACF-3D3404061CEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4726B566-EDE0-4EE5-8E4E-CF8B23FEAF81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="24040" windowHeight="16380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="G2" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="70">
   <si>
     <t>country</t>
   </si>
@@ -209,9 +209,6 @@
     <t>20-030971_G2_Main_Wave3_Merged_FI LI CH_v1_16032021_IntClientUse</t>
   </si>
   <si>
-    <t>20-030971_G1_Merged_Wave6_Final_v1_26032021_IntClientUse</t>
-  </si>
-  <si>
     <t>20-030971_G2_Main_Wave4_Merged_FI LI CH_v1_29032021_IntClientUse</t>
   </si>
   <si>
@@ -240,6 +237,18 @@
   </si>
   <si>
     <t>20-030971_G2_Merged_Wave1_Parents_SL_Final_v1_14042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave6_Final_v2_30042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave7_Final_v2_30042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave4_Merged_SL EL_v1_28042021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave5_Merged_FI LI CH_v1_27042021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -590,14 +599,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -605,7 +614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -613,7 +622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -621,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -629,7 +638,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -637,7 +646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -652,27 +661,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.83203125" style="2"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -711,7 +721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -744,7 +754,7 @@
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -773,11 +783,11 @@
         <v>26</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J55" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <f t="shared" ref="J3:J62" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -810,7 +820,7 @@
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -843,7 +853,7 @@
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -876,7 +886,7 @@
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -909,7 +919,7 @@
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -942,7 +952,7 @@
         <v>pt_sr01_20210118_pA_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -975,7 +985,7 @@
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1008,7 +1018,7 @@
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1051,7 @@
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1084,7 @@
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1107,7 +1117,7 @@
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1140,7 +1150,7 @@
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1173,7 +1183,7 @@
         <v>pt_sr02_20210129_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1206,7 +1216,7 @@
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1239,7 +1249,7 @@
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1272,7 +1282,7 @@
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1315,7 @@
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1338,7 +1348,7 @@
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1371,7 +1381,7 @@
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1404,7 +1414,7 @@
         <v>pt_sr03_20210111_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -1437,7 +1447,7 @@
         <v>at_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1470,7 +1480,7 @@
         <v>dk_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1503,7 +1513,7 @@
         <v>fr_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1536,7 +1546,7 @@
         <v>it_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -1569,7 +1579,7 @@
         <v>pl_sr04_20210226_pC_wv01</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1612,7 @@
         <v>at_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>dk_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1668,7 +1678,7 @@
         <v>fr_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -1701,7 +1711,7 @@
         <v>it_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
@@ -1734,7 +1744,7 @@
         <v>pl_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -1770,7 +1780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -1806,7 +1816,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -1836,7 +1846,7 @@
         <v>at_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -1867,7 +1877,7 @@
         <v>dk_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
@@ -1898,7 +1908,7 @@
         <v>fr_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
@@ -1929,7 +1939,7 @@
         <v>it_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
@@ -1960,7 +1970,7 @@
         <v>pl_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -1991,7 +2001,7 @@
         <v>es_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
@@ -2019,10 +2029,10 @@
       </c>
       <c r="J41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr05_20210325_pA_wv05</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>pt_sr05_20210430_pA_wv05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2042,17 +2052,17 @@
         <v>6</v>
       </c>
       <c r="H42" s="3">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="I42" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="J42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>at_sr07_20210325_pA_wv06</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+        <v>at_sr07_20210430_pA_wv06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2072,17 +2082,17 @@
         <v>6</v>
       </c>
       <c r="H43" s="3">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="I43" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="J43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>dk_sr07_20210325_pA_wv06</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+        <v>dk_sr07_20210430_pA_wv06</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2102,17 +2112,17 @@
         <v>6</v>
       </c>
       <c r="H44" s="3">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="I44" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="J44" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>fr_sr07_20210325_pA_wv06</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+        <v>fr_sr07_20210430_pA_wv06</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2132,17 +2142,17 @@
         <v>6</v>
       </c>
       <c r="H45" s="3">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="I45" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="J45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>it_sr07_20210325_pA_wv06</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+        <v>it_sr07_20210430_pA_wv06</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2162,17 +2172,17 @@
         <v>6</v>
       </c>
       <c r="H46" s="3">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="I46" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="J46" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pl_sr07_20210325_pA_wv06</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+        <v>pl_sr07_20210430_pA_wv06</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -2192,20 +2202,20 @@
         <v>6</v>
       </c>
       <c r="H47" s="3">
-        <v>44280</v>
+        <v>44316</v>
       </c>
       <c r="I47" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="J47" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>es_sr06_20210325_pA_wv06</v>
+        <v>es_sr06_20210430_pA_wv06</v>
       </c>
       <c r="K47" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -2225,10 +2235,10 @@
         <v>6</v>
       </c>
       <c r="H48" s="3">
-        <v>44280</v>
-      </c>
-      <c r="I48" t="s">
-        <v>56</v>
+        <v>44316</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="J48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2238,7 +2248,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -2261,17 +2271,17 @@
         <v>44299</v>
       </c>
       <c r="I49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr07_20210413_pC_wv01</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2294,17 +2304,17 @@
         <v>44299</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pt_sr07_20210413_pC_wv01</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -2327,14 +2337,14 @@
         <v>44299</v>
       </c>
       <c r="I51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -2357,14 +2367,14 @@
         <v>44299</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>22</v>
       </c>
@@ -2387,14 +2397,14 @@
         <v>44299</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2417,14 +2427,14 @@
         <v>44299</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J54" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -2447,11 +2457,221 @@
         <v>44299</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J55" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pl_sr08_19000100_pC_wv02</v>
+        <v>pl_sr08_20210430_pC_wv02</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>4</v>
+      </c>
+      <c r="E56" s="2">
+        <v>9</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56">
+        <v>7</v>
+      </c>
+      <c r="H56" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I56" t="s">
+        <v>67</v>
+      </c>
+      <c r="J56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>at_sr09_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>4</v>
+      </c>
+      <c r="E57" s="2">
+        <v>9</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57">
+        <v>7</v>
+      </c>
+      <c r="H57" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I57" t="s">
+        <v>67</v>
+      </c>
+      <c r="J57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_sr09_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4</v>
+      </c>
+      <c r="E58" s="2">
+        <v>9</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58">
+        <v>7</v>
+      </c>
+      <c r="H58" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I58" t="s">
+        <v>67</v>
+      </c>
+      <c r="J58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr09_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2">
+        <v>4</v>
+      </c>
+      <c r="E59" s="2">
+        <v>9</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59">
+        <v>7</v>
+      </c>
+      <c r="H59" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I59" t="s">
+        <v>67</v>
+      </c>
+      <c r="J59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr09_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2">
+        <v>4</v>
+      </c>
+      <c r="E60" s="2">
+        <v>9</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60">
+        <v>7</v>
+      </c>
+      <c r="H60" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I60" t="s">
+        <v>67</v>
+      </c>
+      <c r="J60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr09_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2">
+        <v>4</v>
+      </c>
+      <c r="E61" s="2">
+        <v>8</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61">
+        <v>7</v>
+      </c>
+      <c r="H61" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I61" t="s">
+        <v>67</v>
+      </c>
+      <c r="J61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr08_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2">
+        <v>4</v>
+      </c>
+      <c r="E62" s="2">
+        <v>8</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62">
+        <v>7</v>
+      </c>
+      <c r="H62" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I62" t="s">
+        <v>67</v>
+      </c>
+      <c r="J62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr08_19000100_pA_wv07</v>
       </c>
     </row>
   </sheetData>
@@ -2462,33 +2682,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:L28"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" activeCellId="1" sqref="G20 G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="71.1640625" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.140625" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>12</v>
@@ -2521,7 +2742,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2555,7 +2776,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2584,12 +2805,12 @@
         <v>34</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J28" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <f t="shared" ref="J3:J33" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>fi_sr01_20210113_pA_wv01</v>
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2623,7 +2844,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -2656,7 +2877,7 @@
         <v>fi_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -2689,7 +2910,7 @@
         <v>ch_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -2718,14 +2939,14 @@
         <v>39</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A7&amp;"_"&amp;"sr"&amp;TEXT(E7,"00")&amp;"_"&amp;YEAR(H8)&amp;TEXT(H8,"MM")&amp;TEXT(H8,"DD")&amp;"_p"&amp;F7&amp;"_wv"&amp;TEXT(G7,"00")&amp;""</f>
         <v>gr_sr01_20210111_pC_wv01</v>
       </c>
       <c r="L7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -2754,11 +2975,11 @@
         <v>39</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A8&amp;"_"&amp;"sr"&amp;TEXT(E8,"00")&amp;"_"&amp;YEAR(H9)&amp;TEXT(H9,"MM")&amp;TEXT(H9,"DD")&amp;"_p"&amp;F8&amp;"_wv"&amp;TEXT(G8,"00")&amp;""</f>
         <v>lt_sr02_20210304_pC_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2787,11 +3008,11 @@
         <v>45</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A9&amp;"_"&amp;"sr"&amp;TEXT(E9,"00")&amp;"_"&amp;YEAR(H10)&amp;TEXT(H10,"MM")&amp;TEXT(H10,"DD")&amp;"_p"&amp;F9&amp;"_wv"&amp;TEXT(G9,"00")&amp;""</f>
         <v>lt_sr03_20210305_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2820,11 +3041,11 @@
         <v>45</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A10&amp;"_"&amp;"sr"&amp;TEXT(E10,"00")&amp;"_"&amp;YEAR(H11)&amp;TEXT(H11,"MM")&amp;TEXT(H11,"DD")&amp;"_p"&amp;F10&amp;"_wv"&amp;TEXT(G10,"00")&amp;""</f>
         <v>fi_sr03_20210306_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -2853,11 +3074,11 @@
         <v>45</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A11&amp;"_"&amp;"sr"&amp;TEXT(E11,"00")&amp;"_"&amp;YEAR(H12)&amp;TEXT(H12,"MM")&amp;TEXT(H12,"DD")&amp;"_p"&amp;F11&amp;"_wv"&amp;TEXT(G11,"00")&amp;""</f>
         <v>ch_sr03_20210307_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2886,48 +3107,48 @@
         <v>46</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>gr_sr02_20210316_pA_wv01</v>
+        <f>A12&amp;"_"&amp;"sr"&amp;TEXT(E12,"00")&amp;"_"&amp;YEAR(H13)&amp;TEXT(H13,"MM")&amp;TEXT(H13,"DD")&amp;"_p"&amp;F12&amp;"_wv"&amp;TEXT(G12,"00")&amp;""</f>
+        <v>gr_sr02_20210329_pA_wv01</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>54</v>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>4</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="4">
-        <v>1</v>
+      <c r="E13" s="2">
+        <v>3</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="4">
-        <v>1</v>
+      <c r="G13" s="2">
+        <v>2</v>
       </c>
       <c r="H13" s="3">
-        <v>44271</v>
+        <v>44284</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>si_sr01_20210316_pA_wv01</v>
+        <f>A13&amp;"_"&amp;"sr"&amp;TEXT(E13,"00")&amp;"_"&amp;YEAR(H14)&amp;TEXT(H14,"MM")&amp;TEXT(H14,"DD")&amp;"_p"&amp;F13&amp;"_wv"&amp;TEXT(G13,"00")&amp;""</f>
+        <v>gr_sr03_20210316_pA_wv02</v>
       </c>
       <c r="L13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -2954,11 +3175,11 @@
         <v>55</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A14&amp;"_"&amp;"sr"&amp;TEXT(E14,"00")&amp;"_"&amp;YEAR(H15)&amp;TEXT(H15,"MM")&amp;TEXT(H15,"DD")&amp;"_p"&amp;F14&amp;"_wv"&amp;TEXT(G14,"00")&amp;""</f>
         <v>fi_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -2985,11 +3206,11 @@
         <v>55</v>
       </c>
       <c r="J15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A15&amp;"_"&amp;"sr"&amp;TEXT(E15,"00")&amp;"_"&amp;YEAR(H16)&amp;TEXT(H16,"MM")&amp;TEXT(H16,"DD")&amp;"_p"&amp;F15&amp;"_wv"&amp;TEXT(G15,"00")&amp;""</f>
         <v>ch_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -3016,11 +3237,11 @@
         <v>55</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A16&amp;"_"&amp;"sr"&amp;TEXT(E16,"00")&amp;"_"&amp;YEAR(H17)&amp;TEXT(H17,"MM")&amp;TEXT(H17,"DD")&amp;"_p"&amp;F16&amp;"_wv"&amp;TEXT(G16,"00")&amp;""</f>
         <v>lt_sr04_20210329_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -3043,14 +3264,14 @@
         <v>44284</v>
       </c>
       <c r="I17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A17&amp;"_"&amp;"sr"&amp;TEXT(E17,"00")&amp;"_"&amp;YEAR(H18)&amp;TEXT(H18,"MM")&amp;TEXT(H18,"DD")&amp;"_p"&amp;F17&amp;"_wv"&amp;TEXT(G17,"00")&amp;""</f>
         <v>fi_sr05_20210329_pA_wv04</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -3073,14 +3294,14 @@
         <v>44284</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A18&amp;"_"&amp;"sr"&amp;TEXT(E18,"00")&amp;"_"&amp;YEAR(H19)&amp;TEXT(H19,"MM")&amp;TEXT(H19,"DD")&amp;"_p"&amp;F18&amp;"_wv"&amp;TEXT(G18,"00")&amp;""</f>
         <v>ch_sr05_20210329_pA_wv04</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -3103,16 +3324,16 @@
         <v>44284</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>lt_sr05_20210329_pA_wv04</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <f>A19&amp;"_"&amp;"sr"&amp;TEXT(E19,"00")&amp;"_"&amp;YEAR(H20)&amp;TEXT(H20,"MM")&amp;TEXT(H20,"DD")&amp;"_p"&amp;F19&amp;"_wv"&amp;TEXT(G19,"00")&amp;""</f>
+        <v>lt_sr05_20210415_pA_wv04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -3121,29 +3342,29 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="H20" s="3">
-        <v>44284</v>
+        <v>44301</v>
       </c>
       <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <f>A20&amp;"_"&amp;"sr"&amp;TEXT(E20,"00")&amp;"_"&amp;YEAR(H21)&amp;TEXT(H21,"MM")&amp;TEXT(H21,"DD")&amp;"_p"&amp;F20&amp;"_wv"&amp;TEXT(G20,"00")&amp;""</f>
+        <v>gr_sr04_20210415_pC_wv02</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>si_sr02_20210329_pA_wv02</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3154,29 +3375,29 @@
         <v>4</v>
       </c>
       <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21">
         <v>3</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
       <c r="H21" s="3">
-        <v>44284</v>
+        <v>44301</v>
       </c>
       <c r="I21" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f>A21&amp;"_"&amp;"sr"&amp;TEXT(E21,"00")&amp;"_"&amp;YEAR(H22)&amp;TEXT(H22,"MM")&amp;TEXT(H22,"DD")&amp;"_p"&amp;F21&amp;"_wv"&amp;TEXT(G21,"00")&amp;""</f>
+        <v>gr_sr05_20210415_pA_wv03</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>gr_sr03_20210415_pA_wv02</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3199,14 +3420,14 @@
         <v>44301</v>
       </c>
       <c r="I22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A22&amp;"_"&amp;"sr"&amp;TEXT(E22,"00")&amp;"_"&amp;YEAR(H23)&amp;TEXT(H23,"MM")&amp;TEXT(H23,"DD")&amp;"_p"&amp;F22&amp;"_wv"&amp;TEXT(G22,"00")&amp;""</f>
         <v>fi_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3229,14 +3450,14 @@
         <v>44301</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A23&amp;"_"&amp;"sr"&amp;TEXT(E23,"00")&amp;"_"&amp;YEAR(H24)&amp;TEXT(H24,"MM")&amp;TEXT(H24,"DD")&amp;"_p"&amp;F23&amp;"_wv"&amp;TEXT(G23,"00")&amp;""</f>
         <v>lt_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -3259,14 +3480,14 @@
         <v>44301</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ch_sr06_20210415_pC_wv02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <f>A24&amp;"_"&amp;"sr"&amp;TEXT(E24,"00")&amp;"_"&amp;YEAR(H25)&amp;TEXT(H25,"MM")&amp;TEXT(H25,"DD")&amp;"_p"&amp;F24&amp;"_wv"&amp;TEXT(G24,"00")&amp;""</f>
+        <v>ch_sr06_20210428_pC_wv02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3277,64 +3498,62 @@
         <v>4</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25" s="3">
-        <v>44301</v>
+        <v>44314</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>gr_sr04_20210415_pC_wv02</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+        <f>A25&amp;"_"&amp;"sr"&amp;TEXT(E25,"00")&amp;"_"&amp;YEAR(H26)&amp;TEXT(H26,"MM")&amp;TEXT(H26,"DD")&amp;"_p"&amp;F25&amp;"_wv"&amp;TEXT(G25,"00")&amp;""</f>
+        <v>gr_sr06_20210316_pA_wv04</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
+      <c r="C26" s="2">
+        <v>4</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="G26" s="4">
         <v>1</v>
       </c>
       <c r="H26" s="3">
-        <v>44301</v>
+        <v>44271</v>
       </c>
       <c r="I26" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>si_sr03_20210415_pC_wv01</v>
+        <f>A26&amp;"_"&amp;"sr"&amp;TEXT(E26,"00")&amp;"_"&amp;YEAR(H27)&amp;TEXT(H27,"MM")&amp;TEXT(H27,"DD")&amp;"_p"&amp;F26&amp;"_wv"&amp;TEXT(G26,"00")&amp;""</f>
+        <v>si_sr01_20210329_pA_wv01</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -3343,29 +3562,29 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="3">
-        <v>44301</v>
+        <v>44284</v>
       </c>
       <c r="I27" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>gr_sr05_20210415_pA_wv03</v>
+        <f>A27&amp;"_"&amp;"sr"&amp;TEXT(E27,"00")&amp;"_"&amp;YEAR(H28)&amp;TEXT(H28,"MM")&amp;TEXT(H28,"DD")&amp;"_p"&amp;F27&amp;"_wv"&amp;TEXT(G27,"00")&amp;""</f>
+        <v>si_sr02_20210415_pA_wv02</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -3376,13 +3595,13 @@
         <v>4</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28" s="3">
         <v>44301</v>
@@ -3391,15 +3610,178 @@
         <v>65</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>si_sr04_19000100_pA_wv03</v>
+        <f>A28&amp;"_"&amp;"sr"&amp;TEXT(E28,"00")&amp;"_"&amp;YEAR(H29)&amp;TEXT(H29,"MM")&amp;TEXT(H29,"DD")&amp;"_p"&amp;F28&amp;"_wv"&amp;TEXT(G28,"00")&amp;""</f>
+        <v>si_sr03_20210415_pC_wv01</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3">
+        <v>44301</v>
+      </c>
+      <c r="I29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="2" t="str">
+        <f>A29&amp;"_"&amp;"sr"&amp;TEXT(E29,"00")&amp;"_"&amp;YEAR(H30)&amp;TEXT(H30,"MM")&amp;TEXT(H30,"DD")&amp;"_p"&amp;F29&amp;"_wv"&amp;TEXT(G29,"00")&amp;""</f>
+        <v>si_sr04_20210428_pA_wv03</v>
+      </c>
+      <c r="L29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3">
+        <v>44314</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <f>A30&amp;"_"&amp;"sr"&amp;TEXT(E30,"00")&amp;"_"&amp;YEAR(H31)&amp;TEXT(H31,"MM")&amp;TEXT(H31,"DD")&amp;"_p"&amp;F30&amp;"_wv"&amp;TEXT(G30,"00")&amp;""</f>
+        <v>si_sr05_20210427_pA_wv04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3">
+        <v>44313</v>
+      </c>
+      <c r="I31" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr07_20210427_pA_wv05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32" s="3">
+        <v>44313</v>
+      </c>
+      <c r="I32" t="s">
+        <v>69</v>
+      </c>
+      <c r="J32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr07_20210427_pA_wv05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33" s="3">
+        <v>44313</v>
+      </c>
+      <c r="I33" t="s">
+        <v>69</v>
+      </c>
+      <c r="J33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr07_19000100_pA_wv05</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L28" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
+  <autoFilter ref="A1:L33" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="gr"/>
+        <filter val="si"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:L30">
+      <sortCondition ref="A1:A33"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add both new and revised data for g2
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27A943E-A83A-43C7-AD50-953BB122D5B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1949D7-B6E8-4D07-8A0A-79EA02268E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="G3" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="76">
   <si>
     <t>country</t>
   </si>
@@ -210,12 +210,6 @@
     <t>20-030971_G2_Main_Wave3_Merged_FI LI CH_v1_16032021_IntClientUse</t>
   </si>
   <si>
-    <t>20-030971_G2_Main_Wave4_Merged_FI LI CH_v1_29032021_IntClientUse</t>
-  </si>
-  <si>
-    <t>20-030971_G2_Main_Wave2_Merged_SL EL_v1_29032021_IntClientUse</t>
-  </si>
-  <si>
     <t>Greece is 2 survey round behind other G2 countries (1 round was unusable)</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t>20-030971_G2_Merged_Wave2_Parents_FI LI CH EL_Final_v1_14042021_IntClientUse</t>
   </si>
   <si>
-    <t>20-030971_G2_Main_Wave3_Merged_SL EL_v1_14042021_IntClientUse</t>
-  </si>
-  <si>
     <t>20-030971_G2_Merged_Wave1_Parents_SL_Final_v1_14042021_IntClientUse</t>
   </si>
   <si>
@@ -246,12 +237,6 @@
     <t>20-030971_G1_Merged_Wave7_Final_v2_30042021_IntClientUse</t>
   </si>
   <si>
-    <t>20-030971_G2_Main_Wave4_Merged_SL EL_v1_28042021_IntClientUse</t>
-  </si>
-  <si>
-    <t>20-030971_G2_Main_Wave5_Merged_FI LI CH_v1_27042021_IntClientUse</t>
-  </si>
-  <si>
     <t>20-030971_G2_Merged_HR EE SK_Wave1_v1_30042021_IntClientUse</t>
   </si>
   <si>
@@ -262,6 +247,27 @@
   </si>
   <si>
     <t>sk</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave2_Merged_SL EL_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave3_Merged_SL EL_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave4_Merged_SL EL_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave5_Merged_SL EL_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave4_Merged_FI LI CH_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave5_Merged_FI LI CH_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave6_Merged_FI LI CH_v2_18052021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -612,14 +618,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -627,7 +633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -635,7 +641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>3</v>
       </c>
@@ -643,7 +649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>4</v>
       </c>
@@ -651,7 +657,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>5</v>
       </c>
@@ -659,7 +665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>6</v>
       </c>
@@ -681,21 +687,21 @@
       <selection pane="bottomLeft" activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.87890625" style="2"/>
+    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
@@ -734,7 +740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -767,7 +773,7 @@
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -800,7 +806,7 @@
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -833,7 +839,7 @@
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -866,7 +872,7 @@
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -899,7 +905,7 @@
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -932,7 +938,7 @@
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -965,7 +971,7 @@
         <v>pt_sr01_20210118_pA_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1097,7 +1103,7 @@
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>pt_sr02_20210129_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1361,7 +1367,7 @@
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1394,7 +1400,7 @@
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>pt_sr03_20210111_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>at_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1493,7 +1499,7 @@
         <v>dk_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1526,7 +1532,7 @@
         <v>fr_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1559,7 +1565,7 @@
         <v>it_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>pl_sr04_20210226_pC_wv01</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>at_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>dk_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>fr_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>it_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
@@ -1757,7 +1763,7 @@
         <v>pl_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -1793,7 +1799,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>at_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>dk_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>fr_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>it_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
@@ -1983,7 +1989,7 @@
         <v>pl_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>es_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>pt_sr05_20210430_pA_wv05</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2068,14 +2074,14 @@
         <v>44316</v>
       </c>
       <c r="I42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2098,14 +2104,14 @@
         <v>44316</v>
       </c>
       <c r="I43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2128,14 +2134,14 @@
         <v>44316</v>
       </c>
       <c r="I44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2158,14 +2164,14 @@
         <v>44316</v>
       </c>
       <c r="I45" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2188,14 +2194,14 @@
         <v>44316</v>
       </c>
       <c r="I46" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J46" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>44316</v>
       </c>
       <c r="I47" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J47" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2228,7 +2234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>44316</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2261,7 +2267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -2284,17 +2290,17 @@
         <v>44299</v>
       </c>
       <c r="I49" t="s">
+        <v>58</v>
+      </c>
+      <c r="J49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr07_20210413_pC_wv01</v>
+      </c>
+      <c r="K49" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J49" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>es_sr07_20210413_pC_wv01</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2317,17 +2323,17 @@
         <v>44299</v>
       </c>
       <c r="I50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr07_20210413_pC_wv01</v>
+      </c>
+      <c r="K50" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J50" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>pt_sr07_20210413_pC_wv01</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -2350,14 +2356,14 @@
         <v>44299</v>
       </c>
       <c r="I51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -2380,14 +2386,14 @@
         <v>44299</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A53" s="2" t="s">
         <v>22</v>
       </c>
@@ -2410,14 +2416,14 @@
         <v>44299</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2440,14 +2446,14 @@
         <v>44299</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J54" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -2470,14 +2476,14 @@
         <v>44299</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J55" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr08_20210430_pC_wv02</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A56" s="2" t="s">
         <v>19</v>
       </c>
@@ -2500,14 +2506,14 @@
         <v>44316</v>
       </c>
       <c r="I56" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57" s="2" t="s">
         <v>20</v>
       </c>
@@ -2530,14 +2536,14 @@
         <v>44316</v>
       </c>
       <c r="I57" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J57" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -2560,14 +2566,14 @@
         <v>44316</v>
       </c>
       <c r="I58" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J58" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -2590,14 +2596,14 @@
         <v>44316</v>
       </c>
       <c r="I59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J59" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A60" s="2" t="s">
         <v>24</v>
       </c>
@@ -2620,14 +2626,14 @@
         <v>44316</v>
       </c>
       <c r="I60" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J60" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
@@ -2650,14 +2656,14 @@
         <v>44316</v>
       </c>
       <c r="I61" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J61" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_sr08_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -2680,7 +2686,7 @@
         <v>44316</v>
       </c>
       <c r="I62" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J62" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2695,33 +2701,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="71.140625" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.41015625" customWidth="1"/>
+    <col min="2" max="2" width="10.41015625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.703125" customWidth="1"/>
+    <col min="4" max="4" width="8.703125" customWidth="1"/>
+    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.41015625" customWidth="1"/>
+    <col min="7" max="7" width="9.29296875" customWidth="1"/>
+    <col min="8" max="8" width="11.703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.1171875" customWidth="1"/>
+    <col min="10" max="10" width="26.1171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>12</v>
@@ -2754,7 +2760,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2788,7 +2794,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2817,12 +2823,12 @@
         <v>34</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J33" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <f t="shared" ref="J3:J38" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>fi_sr01_20210113_pA_wv01</v>
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2856,7 +2862,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>fi_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>ch_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>lt_sr02_20210304_pC_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>lt_sr03_20210305_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>fi_sr03_20210306_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>ch_sr03_20210307_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -3120,13 +3126,13 @@
       </c>
       <c r="J12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>gr_sr02_20210329_pA_wv01</v>
+        <v>gr_sr02_20210519_pA_wv01</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -3147,10 +3153,10 @@
         <v>2</v>
       </c>
       <c r="H13" s="3">
-        <v>44284</v>
+        <v>44335</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="J13" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3160,7 +3166,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>fi_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>ch_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -3250,10 +3256,10 @@
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>lt_sr04_20210329_pA_wv03</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>lt_sr04_20210519_pA_wv03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -3273,17 +3279,17 @@
         <v>4</v>
       </c>
       <c r="H17" s="3">
-        <v>44284</v>
+        <v>44335</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>fi_sr05_20210329_pA_wv04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>fi_sr05_20210519_pA_wv04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -3303,17 +3309,17 @@
         <v>4</v>
       </c>
       <c r="H18" s="3">
-        <v>44284</v>
+        <v>44335</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ch_sr05_20210329_pA_wv04</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>ch_sr05_20210519_pA_wv04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -3333,17 +3339,17 @@
         <v>4</v>
       </c>
       <c r="H19" s="3">
-        <v>44284</v>
+        <v>44335</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="1"/>
         <v>lt_sr05_20210415_pA_wv04</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3366,17 +3372,17 @@
         <v>44301</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>gr_sr04_20210415_pC_wv02</v>
+        <v>gr_sr04_20210519_pC_wv02</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3396,20 +3402,20 @@
         <v>3</v>
       </c>
       <c r="H21" s="3">
-        <v>44301</v>
+        <v>44335</v>
       </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="1"/>
         <v>gr_sr05_20210415_pA_wv03</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3432,14 +3438,14 @@
         <v>44301</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="1"/>
         <v>fi_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3462,14 +3468,14 @@
         <v>44301</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="1"/>
         <v>lt_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -3492,14 +3498,14 @@
         <v>44301</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ch_sr06_20210428_pC_wv02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>ch_sr06_20210519_pC_wv02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3519,10 +3525,10 @@
         <v>4</v>
       </c>
       <c r="H25" s="3">
-        <v>44314</v>
+        <v>44335</v>
       </c>
       <c r="I25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3530,7 +3536,7 @@
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -3557,13 +3563,13 @@
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>si_sr01_20210329_pA_wv01</v>
+        <v>si_sr01_20210519_pA_wv01</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -3583,20 +3589,20 @@
         <v>2</v>
       </c>
       <c r="H27" s="3">
-        <v>44284</v>
+        <v>44335</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="1"/>
         <v>si_sr02_20210415_pA_wv02</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -3619,17 +3625,17 @@
         <v>44301</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>si_sr03_20210415_pC_wv01</v>
+        <v>si_sr03_20210519_pC_wv01</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3649,20 +3655,20 @@
         <v>3</v>
       </c>
       <c r="H29" s="3">
-        <v>44301</v>
+        <v>44335</v>
       </c>
       <c r="I29" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>si_sr04_20210428_pA_wv03</v>
+        <v>si_sr04_20210519_pA_wv03</v>
       </c>
       <c r="L29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3682,17 +3688,17 @@
         <v>4</v>
       </c>
       <c r="H30" s="3">
-        <v>44314</v>
+        <v>44335</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>si_sr05_20210427_pA_wv04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>si_sr05_20210519_pA_wv04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -3712,17 +3718,17 @@
         <v>5</v>
       </c>
       <c r="H31" s="3">
-        <v>44313</v>
+        <v>44335</v>
       </c>
       <c r="I31" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr07_20210427_pA_wv05</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>lt_sr07_20210519_pA_wv05</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -3742,17 +3748,17 @@
         <v>5</v>
       </c>
       <c r="H32" s="3">
-        <v>44313</v>
+        <v>44335</v>
       </c>
       <c r="I32" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>fi_sr07_20210427_pA_wv05</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>fi_sr07_20210519_pA_wv05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -3772,22 +3778,168 @@
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <v>44313</v>
+        <v>44335</v>
       </c>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ch_sr07_19000100_pA_wv05</v>
+        <v>ch_sr07_20210519_pA_wv05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34" s="3">
+        <v>44335</v>
+      </c>
+      <c r="I34" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>gr_sr07_20210519_pA_wv05</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35" s="3">
+        <v>44335</v>
+      </c>
+      <c r="I35" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>si_sr06_20210519_pA_wv05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3">
+        <v>44335</v>
+      </c>
+      <c r="I36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr08_20210519_pA_wv06</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>44335</v>
+      </c>
+      <c r="I37" t="s">
+        <v>75</v>
+      </c>
+      <c r="J37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr08_20210519_pA_wv06</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38">
+        <v>6</v>
+      </c>
+      <c r="H38" s="3">
+        <v>44335</v>
+      </c>
+      <c r="I38" t="s">
+        <v>75</v>
+      </c>
+      <c r="J38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr08_19000100_pA_wv06</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L33" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:L30">
-      <sortCondition ref="A1:A33"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:L38" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3796,23 +3948,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>12</v>
@@ -3845,9 +3997,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3868,16 +4020,16 @@
         <v>44316</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J2" t="str">
         <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
         <v>hr_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3898,16 +4050,16 @@
         <v>44316</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>ee_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3928,7 +4080,7 @@
         <v>44316</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J4" s="2" t="str">
         <f>A4&amp;"_"&amp;"sr"&amp;TEXT(E4,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F4&amp;"_wv"&amp;TEXT(G4,"00")&amp;""</f>

</xml_diff>

<commit_message>
add new g1g2g3 data
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1949D7-B6E8-4D07-8A0A-79EA02268E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77937B2-AF0C-41B8-A2ED-DD88E23DD1AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="G3" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="80">
   <si>
     <t>country</t>
   </si>
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t>20-030971_G2_Main_Wave6_Merged_FI LI CH_v2_18052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave6_Merged_SL EL_v1_25052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave7_Merged_FI LI CH_v1_21052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971-01_G1_PT&amp;ES_Wave2_Parents_Final_v1_21052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave2_v1_21052021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -618,14 +630,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -633,7 +645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -641,7 +653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -649,7 +661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -657,7 +669,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -665,7 +677,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -680,23 +692,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.87890625" style="2"/>
-    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.29296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,7 +752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -773,7 +785,7 @@
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -806,7 +818,7 @@
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -839,7 +851,7 @@
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -872,7 +884,7 @@
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -905,7 +917,7 @@
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -938,7 +950,7 @@
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -971,7 +983,7 @@
         <v>pt_sr01_20210118_pA_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1004,7 +1016,7 @@
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1037,7 +1049,7 @@
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1070,7 +1082,7 @@
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1169,7 +1181,7 @@
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>pt_sr02_20210129_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1235,7 +1247,7 @@
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1268,7 +1280,7 @@
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1400,7 +1412,7 @@
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1433,7 +1445,7 @@
         <v>pt_sr03_20210111_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -1466,7 +1478,7 @@
         <v>at_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1499,7 +1511,7 @@
         <v>dk_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1532,7 +1544,7 @@
         <v>fr_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1565,7 +1577,7 @@
         <v>it_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -1598,7 +1610,7 @@
         <v>pl_sr04_20210226_pC_wv01</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1631,7 +1643,7 @@
         <v>at_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1664,7 +1676,7 @@
         <v>dk_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>fr_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -1730,7 +1742,7 @@
         <v>it_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
@@ -1763,7 +1775,7 @@
         <v>pl_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -1799,7 +1811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -1835,7 +1847,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -1865,7 +1877,7 @@
         <v>at_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -1896,7 +1908,7 @@
         <v>dk_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
@@ -1927,7 +1939,7 @@
         <v>fr_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
@@ -1958,7 +1970,7 @@
         <v>it_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
@@ -1989,7 +2001,7 @@
         <v>pl_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -2020,7 +2032,7 @@
         <v>es_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
@@ -2051,7 +2063,7 @@
         <v>pt_sr05_20210430_pA_wv05</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2081,7 +2093,7 @@
         <v>at_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2111,7 +2123,7 @@
         <v>dk_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2141,7 +2153,7 @@
         <v>fr_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2171,7 +2183,7 @@
         <v>it_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2201,7 +2213,7 @@
         <v>pl_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -2300,7 +2312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2333,7 +2345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -2363,7 +2375,7 @@
         <v>at_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -2393,7 +2405,7 @@
         <v>dk_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>22</v>
       </c>
@@ -2423,7 +2435,7 @@
         <v>fr_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2453,7 +2465,7 @@
         <v>it_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -2483,7 +2495,7 @@
         <v>pl_sr08_20210430_pC_wv02</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>19</v>
       </c>
@@ -2513,7 +2525,7 @@
         <v>at_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>20</v>
       </c>
@@ -2543,7 +2555,7 @@
         <v>dk_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -2573,7 +2585,7 @@
         <v>fr_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -2603,7 +2615,7 @@
         <v>it_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>24</v>
       </c>
@@ -2633,7 +2645,7 @@
         <v>pl_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
@@ -2663,7 +2675,7 @@
         <v>es_sr08_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -2690,7 +2702,59 @@
       </c>
       <c r="J62" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr08_19000100_pA_wv07</v>
+        <v>pt_sr08_20210521_pA_wv07</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="E63">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+      <c r="H63" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>9</v>
+      </c>
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="H64" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I64" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2701,28 +2765,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.41015625" customWidth="1"/>
-    <col min="2" max="2" width="10.41015625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.703125" customWidth="1"/>
-    <col min="4" max="4" width="8.703125" customWidth="1"/>
-    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.41015625" customWidth="1"/>
-    <col min="7" max="7" width="9.29296875" customWidth="1"/>
-    <col min="8" max="8" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="71.1171875" customWidth="1"/>
-    <col min="10" max="10" width="26.1171875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2760,7 +2824,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2794,7 +2858,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2823,12 +2887,12 @@
         <v>34</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J38" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <f t="shared" ref="J3:J43" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>fi_sr01_20210113_pA_wv01</v>
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2862,7 +2926,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -2895,7 +2959,7 @@
         <v>fi_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -2928,7 +2992,7 @@
         <v>ch_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -2964,7 +3028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -2997,7 +3061,7 @@
         <v>lt_sr02_20210304_pC_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3030,7 +3094,7 @@
         <v>lt_sr03_20210305_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -3063,7 +3127,7 @@
         <v>fi_sr03_20210306_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3096,7 +3160,7 @@
         <v>ch_sr03_20210307_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -3132,7 +3196,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -3166,7 +3230,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3197,7 +3261,7 @@
         <v>fi_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -3228,7 +3292,7 @@
         <v>ch_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -3259,7 +3323,7 @@
         <v>lt_sr04_20210519_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -3289,7 +3353,7 @@
         <v>fi_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -3319,7 +3383,7 @@
         <v>ch_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -3349,7 +3413,7 @@
         <v>lt_sr05_20210415_pA_wv04</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3382,7 +3446,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3415,7 +3479,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3445,7 +3509,7 @@
         <v>fi_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3475,7 +3539,7 @@
         <v>lt_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -3505,7 +3569,7 @@
         <v>ch_sr06_20210519_pC_wv02</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3536,7 +3600,7 @@
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -3569,7 +3633,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -3602,7 +3666,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -3635,7 +3699,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3668,7 +3732,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3698,7 +3762,7 @@
         <v>si_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -3728,7 +3792,7 @@
         <v>lt_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -3758,7 +3822,7 @@
         <v>fi_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -3788,7 +3852,7 @@
         <v>ch_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3818,7 +3882,7 @@
         <v>gr_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3848,7 +3912,7 @@
         <v>si_sr06_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3878,7 +3942,7 @@
         <v>fi_sr08_20210519_pA_wv06</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3908,7 +3972,7 @@
         <v>lt_sr08_20210519_pA_wv06</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -3935,31 +3999,181 @@
       </c>
       <c r="J38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ch_sr08_19000100_pA_wv06</v>
+        <v>ch_sr08_20210525_pA_wv06</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39" s="3">
+        <v>44341</v>
+      </c>
+      <c r="I39" t="s">
+        <v>76</v>
+      </c>
+      <c r="J39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>gr_sr08_20210525_pA_wv06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>6</v>
+      </c>
+      <c r="H40" s="3">
+        <v>44341</v>
+      </c>
+      <c r="I40" t="s">
+        <v>76</v>
+      </c>
+      <c r="J40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>si_sr08_20210521_pA_wv06</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>9</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="H41" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I41" t="s">
+        <v>77</v>
+      </c>
+      <c r="J41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr09_20210521_pA_wv07</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>9</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="H42" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I42" t="s">
+        <v>77</v>
+      </c>
+      <c r="J42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr09_20210521_pA_wv07</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>9</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43">
+        <v>7</v>
+      </c>
+      <c r="H43" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I43" t="s">
+        <v>77</v>
+      </c>
+      <c r="J43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr09_19000100_pA_wv07</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L38" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
+  <autoFilter ref="A1:L43" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3997,7 +4211,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -4027,7 +4241,7 @@
         <v>hr_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -4057,7 +4271,7 @@
         <v>ee_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -4085,6 +4299,96 @@
       <c r="J4" s="2" t="str">
         <f>A4&amp;"_"&amp;"sr"&amp;TEXT(E4,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F4&amp;"_wv"&amp;TEXT(G4,"00")&amp;""</f>
         <v>sk_sr01_20210430_pA_wv01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f>A5&amp;"_"&amp;"sr"&amp;TEXT(E5,"00")&amp;"_"&amp;YEAR(H5)&amp;TEXT(H5,"MM")&amp;TEXT(H5,"DD")&amp;"_p"&amp;F5&amp;"_wv"&amp;TEXT(G5,"00")&amp;""</f>
+        <v>hr_sr02_20210521_pA_wv02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>A6&amp;"_"&amp;"sr"&amp;TEXT(E6,"00")&amp;"_"&amp;YEAR(H6)&amp;TEXT(H6,"MM")&amp;TEXT(H6,"DD")&amp;"_p"&amp;F6&amp;"_wv"&amp;TEXT(G6,"00")&amp;""</f>
+        <v>ee_sr02_20210521_pA_wv02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f>A7&amp;"_"&amp;"sr"&amp;TEXT(E7,"00")&amp;"_"&amp;YEAR(H7)&amp;TEXT(H7,"MM")&amp;TEXT(H7,"DD")&amp;"_p"&amp;F7&amp;"_wv"&amp;TEXT(G7,"00")&amp;""</f>
+        <v>sk_sr02_20210521_pA_wv02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new g2 g3 countries
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77937B2-AF0C-41B8-A2ED-DD88E23DD1AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122D76AD-56E2-4A83-A81B-AAD48442AAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="G3" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="82">
   <si>
     <t>country</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>20-030971_G3_Merged_HR EE SK_Wave2_v1_21052021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave7_Merged_SL EL_v1_14062021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_PARENTS_HR EE SK_Wave1_v1_22062021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -630,14 +636,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -645,7 +651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -653,7 +659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>3</v>
       </c>
@@ -661,7 +667,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>4</v>
       </c>
@@ -669,7 +675,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>5</v>
       </c>
@@ -677,7 +683,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>6</v>
       </c>
@@ -694,21 +700,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.87890625" style="2"/>
+    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -780,12 +786,12 @@
       <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="str">
-        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
+      <c r="J2" s="2" t="str">
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -814,11 +820,11 @@
         <v>26</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J62" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <f t="shared" ref="J3:J64" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -851,7 +857,7 @@
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -884,7 +890,7 @@
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -917,7 +923,7 @@
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -950,7 +956,7 @@
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -980,10 +986,10 @@
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr01_20210118_pA_wv01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>pt_sr01_20210111_pA_wv01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1211,10 +1217,10 @@
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr02_20210129_pA_wv02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>pt_sr02_20210118_pA_wv02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1313,7 +1319,7 @@
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1442,10 +1448,10 @@
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr03_20210111_pA_wv03</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>pt_sr03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>at_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>dk_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>fr_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1577,7 +1583,7 @@
         <v>it_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -1607,10 +1613,10 @@
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pl_sr04_20210226_pC_wv01</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>pl_sr04_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>at_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1676,7 +1682,7 @@
         <v>dk_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>fr_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>it_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>pl_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -1811,7 +1817,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -1841,13 +1847,13 @@
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr04_20210316_pA_wv04</v>
+        <v>pt_sr04_20210226_pA_wv04</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>at_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>dk_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>fr_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>it_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
@@ -2001,7 +2007,7 @@
         <v>pl_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -2032,7 +2038,7 @@
         <v>es_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
@@ -2060,10 +2066,10 @@
       </c>
       <c r="J41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr05_20210430_pA_wv05</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>pt_sr05_20210316_pA_wv05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>at_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2123,7 +2129,7 @@
         <v>dk_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2153,7 +2159,7 @@
         <v>fr_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2183,7 +2189,7 @@
         <v>it_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2213,7 +2219,7 @@
         <v>pl_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -2273,13 +2279,13 @@
       </c>
       <c r="J48" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr06_20210413_pA_wv06</v>
+        <v>pt_sr06_20210430_pA_wv06</v>
       </c>
       <c r="K48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -2312,7 +2318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -2375,7 +2381,7 @@
         <v>at_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>dk_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A53" s="2" t="s">
         <v>22</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>fr_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2465,7 +2471,7 @@
         <v>it_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -2492,10 +2498,10 @@
       </c>
       <c r="J55" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pl_sr08_20210430_pC_wv02</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>pl_sr08_20210413_pC_wv02</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A56" s="2" t="s">
         <v>19</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>at_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A57" s="2" t="s">
         <v>20</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>dk_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -2585,7 +2591,7 @@
         <v>fr_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>it_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A60" s="2" t="s">
         <v>24</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>pl_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
@@ -2675,7 +2681,7 @@
         <v>es_sr08_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -2702,10 +2708,10 @@
       </c>
       <c r="J62" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_sr08_20210521_pA_wv07</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+        <v>pt_sr08_20210430_pA_wv07</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
         <v>21</v>
       </c>
@@ -2730,8 +2736,12 @@
       <c r="I63" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr09_20210521_pC_wv02</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
         <v>25</v>
       </c>
@@ -2755,6 +2765,10 @@
       </c>
       <c r="I64" t="s">
         <v>78</v>
+      </c>
+      <c r="J64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr09_20210521_pC_wv02</v>
       </c>
     </row>
   </sheetData>
@@ -2765,28 +2779,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="71.140625" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.41015625" customWidth="1"/>
+    <col min="2" max="2" width="10.41015625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.703125" customWidth="1"/>
+    <col min="4" max="4" width="8.703125" customWidth="1"/>
+    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.41015625" customWidth="1"/>
+    <col min="7" max="7" width="9.29296875" customWidth="1"/>
+    <col min="8" max="8" width="11.703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.1171875" customWidth="1"/>
+    <col min="10" max="10" width="26.1171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2824,7 +2838,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2853,12 +2867,12 @@
         <v>34</v>
       </c>
       <c r="J2" s="2" t="str">
-        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
-        <v>lt_sr01_20210112_pA_wv01</v>
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
+        <v>lt_sr01_20210111_pA_wv01</v>
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2887,12 +2901,12 @@
         <v>34</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J43" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
-        <v>fi_sr01_20210113_pA_wv01</v>
+        <f>A3&amp;"_"&amp;"sr"&amp;TEXT(E3,"00")&amp;"_"&amp;YEAR(H3)&amp;TEXT(H3,"MM")&amp;TEXT(H3,"DD")&amp;"_p"&amp;F3&amp;"_wv"&amp;TEXT(G3,"00")&amp;""</f>
+        <v>fi_sr01_20210112_pA_wv01</v>
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2921,12 +2935,12 @@
         <v>34</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ch_sr01_20210112_pA_wv01</v>
+        <f>A4&amp;"_"&amp;"sr"&amp;TEXT(E4,"00")&amp;"_"&amp;YEAR(H4)&amp;TEXT(H4,"MM")&amp;TEXT(H4,"DD")&amp;"_p"&amp;F4&amp;"_wv"&amp;TEXT(G4,"00")&amp;""</f>
+        <v>ch_sr01_20210113_pA_wv01</v>
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -2955,11 +2969,11 @@
         <v>39</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>fi_sr02_20210113_pC_wv01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A5&amp;"_"&amp;"sr"&amp;TEXT(E5,"00")&amp;"_"&amp;YEAR(H5)&amp;TEXT(H5,"MM")&amp;TEXT(H5,"DD")&amp;"_p"&amp;F5&amp;"_wv"&amp;TEXT(G5,"00")&amp;""</f>
+        <v>fi_sr02_20210112_pC_wv01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -2988,11 +3002,11 @@
         <v>39</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A6&amp;"_"&amp;"sr"&amp;TEXT(E6,"00")&amp;"_"&amp;YEAR(H6)&amp;TEXT(H6,"MM")&amp;TEXT(H6,"DD")&amp;"_p"&amp;F6&amp;"_wv"&amp;TEXT(G6,"00")&amp;""</f>
         <v>ch_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -3021,14 +3035,14 @@
         <v>39</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" ref="J7:J30" si="1">A7&amp;"_"&amp;"sr"&amp;TEXT(E7,"00")&amp;"_"&amp;YEAR(H8)&amp;TEXT(H8,"MM")&amp;TEXT(H8,"DD")&amp;"_p"&amp;F7&amp;"_wv"&amp;TEXT(G7,"00")&amp;""</f>
-        <v>gr_sr01_20210111_pC_wv01</v>
+        <f>A7&amp;"_"&amp;"sr"&amp;TEXT(E7,"00")&amp;"_"&amp;YEAR(H7)&amp;TEXT(H7,"MM")&amp;TEXT(H7,"DD")&amp;"_p"&amp;F7&amp;"_wv"&amp;TEXT(G7,"00")&amp;""</f>
+        <v>gr_sr01_20210113_pC_wv01</v>
       </c>
       <c r="L7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -3057,11 +3071,11 @@
         <v>39</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>lt_sr02_20210304_pC_wv01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A8&amp;"_"&amp;"sr"&amp;TEXT(E8,"00")&amp;"_"&amp;YEAR(H8)&amp;TEXT(H8,"MM")&amp;TEXT(H8,"DD")&amp;"_p"&amp;F8&amp;"_wv"&amp;TEXT(G8,"00")&amp;""</f>
+        <v>lt_sr02_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3090,11 +3104,11 @@
         <v>45</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>lt_sr03_20210305_pA_wv02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A9&amp;"_"&amp;"sr"&amp;TEXT(E9,"00")&amp;"_"&amp;YEAR(H9)&amp;TEXT(H9,"MM")&amp;TEXT(H9,"DD")&amp;"_p"&amp;F9&amp;"_wv"&amp;TEXT(G9,"00")&amp;""</f>
+        <v>lt_sr03_20210304_pA_wv02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -3123,11 +3137,11 @@
         <v>45</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>fi_sr03_20210306_pA_wv02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A10&amp;"_"&amp;"sr"&amp;TEXT(E10,"00")&amp;"_"&amp;YEAR(H10)&amp;TEXT(H10,"MM")&amp;TEXT(H10,"DD")&amp;"_p"&amp;F10&amp;"_wv"&amp;TEXT(G10,"00")&amp;""</f>
+        <v>fi_sr03_20210305_pA_wv02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3156,11 +3170,11 @@
         <v>45</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>ch_sr03_20210307_pA_wv02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A11&amp;"_"&amp;"sr"&amp;TEXT(E11,"00")&amp;"_"&amp;YEAR(H11)&amp;TEXT(H11,"MM")&amp;TEXT(H11,"DD")&amp;"_p"&amp;F11&amp;"_wv"&amp;TEXT(G11,"00")&amp;""</f>
+        <v>ch_sr03_20210306_pA_wv02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -3189,14 +3203,14 @@
         <v>46</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>gr_sr02_20210519_pA_wv01</v>
+        <f>A12&amp;"_"&amp;"sr"&amp;TEXT(E12,"00")&amp;"_"&amp;YEAR(H12)&amp;TEXT(H12,"MM")&amp;TEXT(H12,"DD")&amp;"_p"&amp;F12&amp;"_wv"&amp;TEXT(G12,"00")&amp;""</f>
+        <v>gr_sr02_20210307_pA_wv01</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -3223,14 +3237,14 @@
         <v>69</v>
       </c>
       <c r="J13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>gr_sr03_20210316_pA_wv02</v>
+        <f>A13&amp;"_"&amp;"sr"&amp;TEXT(E13,"00")&amp;"_"&amp;YEAR(H13)&amp;TEXT(H13,"MM")&amp;TEXT(H13,"DD")&amp;"_p"&amp;F13&amp;"_wv"&amp;TEXT(G13,"00")&amp;""</f>
+        <v>gr_sr03_20210519_pA_wv02</v>
       </c>
       <c r="L13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -3257,11 +3271,11 @@
         <v>55</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A14&amp;"_"&amp;"sr"&amp;TEXT(E14,"00")&amp;"_"&amp;YEAR(H14)&amp;TEXT(H14,"MM")&amp;TEXT(H14,"DD")&amp;"_p"&amp;F14&amp;"_wv"&amp;TEXT(G14,"00")&amp;""</f>
         <v>fi_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -3288,11 +3302,11 @@
         <v>55</v>
       </c>
       <c r="J15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A15&amp;"_"&amp;"sr"&amp;TEXT(E15,"00")&amp;"_"&amp;YEAR(H15)&amp;TEXT(H15,"MM")&amp;TEXT(H15,"DD")&amp;"_p"&amp;F15&amp;"_wv"&amp;TEXT(G15,"00")&amp;""</f>
         <v>ch_sr04_20210316_pA_wv03</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -3319,11 +3333,11 @@
         <v>55</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>lt_sr04_20210519_pA_wv03</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A16&amp;"_"&amp;"sr"&amp;TEXT(E16,"00")&amp;"_"&amp;YEAR(H16)&amp;TEXT(H16,"MM")&amp;TEXT(H16,"DD")&amp;"_p"&amp;F16&amp;"_wv"&amp;TEXT(G16,"00")&amp;""</f>
+        <v>lt_sr04_20210316_pA_wv03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -3349,11 +3363,11 @@
         <v>73</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A17&amp;"_"&amp;"sr"&amp;TEXT(E17,"00")&amp;"_"&amp;YEAR(H17)&amp;TEXT(H17,"MM")&amp;TEXT(H17,"DD")&amp;"_p"&amp;F17&amp;"_wv"&amp;TEXT(G17,"00")&amp;""</f>
         <v>fi_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
@@ -3379,11 +3393,11 @@
         <v>73</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A18&amp;"_"&amp;"sr"&amp;TEXT(E18,"00")&amp;"_"&amp;YEAR(H18)&amp;TEXT(H18,"MM")&amp;TEXT(H18,"DD")&amp;"_p"&amp;F18&amp;"_wv"&amp;TEXT(G18,"00")&amp;""</f>
         <v>ch_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -3409,11 +3423,11 @@
         <v>73</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>lt_sr05_20210415_pA_wv04</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A19&amp;"_"&amp;"sr"&amp;TEXT(E19,"00")&amp;"_"&amp;YEAR(H19)&amp;TEXT(H19,"MM")&amp;TEXT(H19,"DD")&amp;"_p"&amp;F19&amp;"_wv"&amp;TEXT(G19,"00")&amp;""</f>
+        <v>lt_sr05_20210519_pA_wv04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3439,14 +3453,14 @@
         <v>61</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>gr_sr04_20210519_pC_wv02</v>
+        <f>A20&amp;"_"&amp;"sr"&amp;TEXT(E20,"00")&amp;"_"&amp;YEAR(H20)&amp;TEXT(H20,"MM")&amp;TEXT(H20,"DD")&amp;"_p"&amp;F20&amp;"_wv"&amp;TEXT(G20,"00")&amp;""</f>
+        <v>gr_sr04_20210415_pC_wv02</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3472,14 +3486,14 @@
         <v>70</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>gr_sr05_20210415_pA_wv03</v>
+        <f>A21&amp;"_"&amp;"sr"&amp;TEXT(E21,"00")&amp;"_"&amp;YEAR(H21)&amp;TEXT(H21,"MM")&amp;TEXT(H21,"DD")&amp;"_p"&amp;F21&amp;"_wv"&amp;TEXT(G21,"00")&amp;""</f>
+        <v>gr_sr05_20210519_pA_wv03</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3505,11 +3519,11 @@
         <v>61</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A22&amp;"_"&amp;"sr"&amp;TEXT(E22,"00")&amp;"_"&amp;YEAR(H22)&amp;TEXT(H22,"MM")&amp;TEXT(H22,"DD")&amp;"_p"&amp;F22&amp;"_wv"&amp;TEXT(G22,"00")&amp;""</f>
         <v>fi_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3535,11 +3549,11 @@
         <v>61</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A23&amp;"_"&amp;"sr"&amp;TEXT(E23,"00")&amp;"_"&amp;YEAR(H23)&amp;TEXT(H23,"MM")&amp;TEXT(H23,"DD")&amp;"_p"&amp;F23&amp;"_wv"&amp;TEXT(G23,"00")&amp;""</f>
         <v>lt_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -3565,11 +3579,11 @@
         <v>61</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>ch_sr06_20210519_pC_wv02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <f>A24&amp;"_"&amp;"sr"&amp;TEXT(E24,"00")&amp;"_"&amp;YEAR(H24)&amp;TEXT(H24,"MM")&amp;TEXT(H24,"DD")&amp;"_p"&amp;F24&amp;"_wv"&amp;TEXT(G24,"00")&amp;""</f>
+        <v>ch_sr06_20210415_pC_wv02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3595,12 +3609,12 @@
         <v>71</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>gr_sr06_20210316_pA_wv04</v>
+        <f>A25&amp;"_"&amp;"sr"&amp;TEXT(E25,"00")&amp;"_"&amp;YEAR(H25)&amp;TEXT(H25,"MM")&amp;TEXT(H25,"DD")&amp;"_p"&amp;F25&amp;"_wv"&amp;TEXT(G25,"00")&amp;""</f>
+        <v>gr_sr06_20210519_pA_wv04</v>
       </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -3626,14 +3640,14 @@
         <v>51</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>si_sr01_20210519_pA_wv01</v>
+        <f>A26&amp;"_"&amp;"sr"&amp;TEXT(E26,"00")&amp;"_"&amp;YEAR(H26)&amp;TEXT(H26,"MM")&amp;TEXT(H26,"DD")&amp;"_p"&amp;F26&amp;"_wv"&amp;TEXT(G26,"00")&amp;""</f>
+        <v>si_sr01_20210316_pA_wv01</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -3659,14 +3673,14 @@
         <v>69</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>si_sr02_20210415_pA_wv02</v>
+        <f>A27&amp;"_"&amp;"sr"&amp;TEXT(E27,"00")&amp;"_"&amp;YEAR(H27)&amp;TEXT(H27,"MM")&amp;TEXT(H27,"DD")&amp;"_p"&amp;F27&amp;"_wv"&amp;TEXT(G27,"00")&amp;""</f>
+        <v>si_sr02_20210519_pA_wv02</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -3692,14 +3706,14 @@
         <v>62</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>si_sr03_20210519_pC_wv01</v>
+        <f>A28&amp;"_"&amp;"sr"&amp;TEXT(E28,"00")&amp;"_"&amp;YEAR(H28)&amp;TEXT(H28,"MM")&amp;TEXT(H28,"DD")&amp;"_p"&amp;F28&amp;"_wv"&amp;TEXT(G28,"00")&amp;""</f>
+        <v>si_sr03_20210415_pC_wv01</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -3725,14 +3739,14 @@
         <v>70</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A29&amp;"_"&amp;"sr"&amp;TEXT(E29,"00")&amp;"_"&amp;YEAR(H29)&amp;TEXT(H29,"MM")&amp;TEXT(H29,"DD")&amp;"_p"&amp;F29&amp;"_wv"&amp;TEXT(G29,"00")&amp;""</f>
         <v>si_sr04_20210519_pA_wv03</v>
       </c>
       <c r="L29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -3758,11 +3772,11 @@
         <v>71</v>
       </c>
       <c r="J30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A30&amp;"_"&amp;"sr"&amp;TEXT(E30,"00")&amp;"_"&amp;YEAR(H30)&amp;TEXT(H30,"MM")&amp;TEXT(H30,"DD")&amp;"_p"&amp;F30&amp;"_wv"&amp;TEXT(G30,"00")&amp;""</f>
         <v>si_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -3788,11 +3802,11 @@
         <v>74</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A31&amp;"_"&amp;"sr"&amp;TEXT(E31,"00")&amp;"_"&amp;YEAR(H31)&amp;TEXT(H31,"MM")&amp;TEXT(H31,"DD")&amp;"_p"&amp;F31&amp;"_wv"&amp;TEXT(G31,"00")&amp;""</f>
         <v>lt_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -3818,11 +3832,11 @@
         <v>74</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A32&amp;"_"&amp;"sr"&amp;TEXT(E32,"00")&amp;"_"&amp;YEAR(H32)&amp;TEXT(H32,"MM")&amp;TEXT(H32,"DD")&amp;"_p"&amp;F32&amp;"_wv"&amp;TEXT(G32,"00")&amp;""</f>
         <v>fi_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -3848,11 +3862,11 @@
         <v>74</v>
       </c>
       <c r="J33" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A33&amp;"_"&amp;"sr"&amp;TEXT(E33,"00")&amp;"_"&amp;YEAR(H33)&amp;TEXT(H33,"MM")&amp;TEXT(H33,"DD")&amp;"_p"&amp;F33&amp;"_wv"&amp;TEXT(G33,"00")&amp;""</f>
         <v>ch_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3878,11 +3892,11 @@
         <v>72</v>
       </c>
       <c r="J34" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A34&amp;"_"&amp;"sr"&amp;TEXT(E34,"00")&amp;"_"&amp;YEAR(H34)&amp;TEXT(H34,"MM")&amp;TEXT(H34,"DD")&amp;"_p"&amp;F34&amp;"_wv"&amp;TEXT(G34,"00")&amp;""</f>
         <v>gr_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3908,11 +3922,11 @@
         <v>72</v>
       </c>
       <c r="J35" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A35&amp;"_"&amp;"sr"&amp;TEXT(E35,"00")&amp;"_"&amp;YEAR(H35)&amp;TEXT(H35,"MM")&amp;TEXT(H35,"DD")&amp;"_p"&amp;F35&amp;"_wv"&amp;TEXT(G35,"00")&amp;""</f>
         <v>si_sr06_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3938,11 +3952,11 @@
         <v>75</v>
       </c>
       <c r="J36" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A36&amp;"_"&amp;"sr"&amp;TEXT(E36,"00")&amp;"_"&amp;YEAR(H36)&amp;TEXT(H36,"MM")&amp;TEXT(H36,"DD")&amp;"_p"&amp;F36&amp;"_wv"&amp;TEXT(G36,"00")&amp;""</f>
         <v>fi_sr08_20210519_pA_wv06</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3968,11 +3982,11 @@
         <v>75</v>
       </c>
       <c r="J37" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A37&amp;"_"&amp;"sr"&amp;TEXT(E37,"00")&amp;"_"&amp;YEAR(H37)&amp;TEXT(H37,"MM")&amp;TEXT(H37,"DD")&amp;"_p"&amp;F37&amp;"_wv"&amp;TEXT(G37,"00")&amp;""</f>
         <v>lt_sr08_20210519_pA_wv06</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -3998,11 +4012,11 @@
         <v>75</v>
       </c>
       <c r="J38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ch_sr08_20210525_pA_wv06</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <f>A38&amp;"_"&amp;"sr"&amp;TEXT(E38,"00")&amp;"_"&amp;YEAR(H38)&amp;TEXT(H38,"MM")&amp;TEXT(H38,"DD")&amp;"_p"&amp;F38&amp;"_wv"&amp;TEXT(G38,"00")&amp;""</f>
+        <v>ch_sr08_20210519_pA_wv06</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -4028,11 +4042,11 @@
         <v>76</v>
       </c>
       <c r="J39" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A39&amp;"_"&amp;"sr"&amp;TEXT(E39,"00")&amp;"_"&amp;YEAR(H39)&amp;TEXT(H39,"MM")&amp;TEXT(H39,"DD")&amp;"_p"&amp;F39&amp;"_wv"&amp;TEXT(G39,"00")&amp;""</f>
         <v>gr_sr08_20210525_pA_wv06</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -4043,7 +4057,7 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>9</v>
@@ -4058,11 +4072,11 @@
         <v>76</v>
       </c>
       <c r="J40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>si_sr08_20210521_pA_wv06</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <f>A40&amp;"_"&amp;"sr"&amp;TEXT(E40,"00")&amp;"_"&amp;YEAR(H40)&amp;TEXT(H40,"MM")&amp;TEXT(H40,"DD")&amp;"_p"&amp;F40&amp;"_wv"&amp;TEXT(G40,"00")&amp;""</f>
+        <v>si_sr07_20210525_pA_wv06</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -4088,11 +4102,11 @@
         <v>77</v>
       </c>
       <c r="J41" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A41&amp;"_"&amp;"sr"&amp;TEXT(E41,"00")&amp;"_"&amp;YEAR(H41)&amp;TEXT(H41,"MM")&amp;TEXT(H41,"DD")&amp;"_p"&amp;F41&amp;"_wv"&amp;TEXT(G41,"00")&amp;""</f>
         <v>fi_sr09_20210521_pA_wv07</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -4118,11 +4132,11 @@
         <v>77</v>
       </c>
       <c r="J42" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A42&amp;"_"&amp;"sr"&amp;TEXT(E42,"00")&amp;"_"&amp;YEAR(H42)&amp;TEXT(H42,"MM")&amp;TEXT(H42,"DD")&amp;"_p"&amp;F42&amp;"_wv"&amp;TEXT(G42,"00")&amp;""</f>
         <v>lt_sr09_20210521_pA_wv07</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -4148,32 +4162,92 @@
         <v>77</v>
       </c>
       <c r="J43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>ch_sr09_19000100_pA_wv07</v>
+        <f>A43&amp;"_"&amp;"sr"&amp;TEXT(E43,"00")&amp;"_"&amp;YEAR(H43)&amp;TEXT(H43,"MM")&amp;TEXT(H43,"DD")&amp;"_p"&amp;F43&amp;"_wv"&amp;TEXT(G43,"00")&amp;""</f>
+        <v>ch_sr09_20210521_pA_wv07</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44" s="3">
+        <v>44369</v>
+      </c>
+      <c r="I44" t="s">
+        <v>80</v>
+      </c>
+      <c r="J44" t="str">
+        <f>A44&amp;"_"&amp;"sr"&amp;TEXT(E44,"00")&amp;"_"&amp;YEAR(H44)&amp;TEXT(H44,"MM")&amp;TEXT(H44,"DD")&amp;"_p"&amp;F44&amp;"_wv"&amp;TEXT(G44,"00")&amp;""</f>
+        <v>si_sr08_20210622_pA_wv07</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>9</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="H45" s="3">
+        <v>44369</v>
+      </c>
+      <c r="I45" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" t="str">
+        <f>A45&amp;"_"&amp;"sr"&amp;TEXT(E45,"00")&amp;"_"&amp;YEAR(H45)&amp;TEXT(H45,"MM")&amp;TEXT(H45,"DD")&amp;"_p"&amp;F45&amp;"_wv"&amp;TEXT(G45,"00")&amp;""</f>
+        <v>gr_sr09_20210622_pA_wv07</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L43" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
+  <autoFilter ref="A1:L45" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4211,7 +4285,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -4241,7 +4315,7 @@
         <v>hr_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -4271,7 +4345,7 @@
         <v>ee_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -4301,7 +4375,7 @@
         <v>sk_sr01_20210430_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -4331,7 +4405,7 @@
         <v>hr_sr02_20210521_pA_wv02</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
@@ -4361,7 +4435,7 @@
         <v>ee_sr02_20210521_pA_wv02</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
@@ -4389,6 +4463,96 @@
       <c r="J7" s="2" t="str">
         <f>A7&amp;"_"&amp;"sr"&amp;TEXT(E7,"00")&amp;"_"&amp;YEAR(H7)&amp;TEXT(H7,"MM")&amp;TEXT(H7,"DD")&amp;"_p"&amp;F7&amp;"_wv"&amp;TEXT(G7,"00")&amp;""</f>
         <v>sk_sr02_20210521_pA_wv02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>44369</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" t="str">
+        <f>A8&amp;"_"&amp;"sr"&amp;TEXT(E8,"00")&amp;"_"&amp;YEAR(H8)&amp;TEXT(H8,"MM")&amp;TEXT(H8,"DD")&amp;"_p"&amp;F8&amp;"_wv"&amp;TEXT(G8,"00")&amp;""</f>
+        <v>hr_sr03_20210622_pC_wv01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>44369</v>
+      </c>
+      <c r="I9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" t="str">
+        <f>A9&amp;"_"&amp;"sr"&amp;TEXT(E9,"00")&amp;"_"&amp;YEAR(H9)&amp;TEXT(H9,"MM")&amp;TEXT(H9,"DD")&amp;"_p"&amp;F9&amp;"_wv"&amp;TEXT(G9,"00")&amp;""</f>
+        <v>ee_sr03_20210622_pC_wv01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>44369</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" t="str">
+        <f>A10&amp;"_"&amp;"sr"&amp;TEXT(E10,"00")&amp;"_"&amp;YEAR(H10)&amp;TEXT(H10,"MM")&amp;TEXT(H10,"DD")&amp;"_p"&amp;F10&amp;"_wv"&amp;TEXT(G10,"00")&amp;""</f>
+        <v>sk_sr03_20210622_pC_wv01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new g2 and g3 data
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4AFD8F-46B3-4696-9A6E-C4115D090C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF854AC8-B5C6-4DFA-88A5-F9663FAC824E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="1410" windowWidth="21600" windowHeight="11070" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="G2_archive" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">G2_archive!$A$1:$M$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'G3'!$A$1:$L$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'G3'!$A$1:$L$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="149">
   <si>
     <t>country</t>
   </si>
@@ -463,6 +463,33 @@
   </si>
   <si>
     <t>20-030971_G3_HU_Wave3_v1_28072021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Wave2_Parents_SL_Final_v1_10072021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave9_(2nd additional)_FI&amp;LI_v1_06082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave10_(3rd additional)_CH_v1_06082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave11_(4th additional)_CH_v1_19082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave4_v1_03082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave6_v1_06082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_MT_Wave2_v1_06082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave7_v1_19082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave5_v1_19082021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -2956,11 +2983,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomLeft" activeCell="H55" sqref="H51:H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,7 +3072,7 @@
         <v>39</v>
       </c>
       <c r="J2" s="2" t="str">
-        <f t="shared" ref="J2:J50" si="0">A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
+        <f t="shared" ref="J2:J55" si="0">A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
         <v>fi_sr02_20210112_pC_wv01</v>
       </c>
     </row>
@@ -4548,8 +4575,158 @@
         <v>ch_sr12_20210723_pB_wv02</v>
       </c>
     </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>9</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51" s="3">
+        <v>44393</v>
+      </c>
+      <c r="I51" t="s">
+        <v>140</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="0"/>
+        <v>si_sr09_20210716_pC_wv02</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4">
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52" s="3">
+        <v>44431</v>
+      </c>
+      <c r="I52" t="s">
+        <v>141</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr11_20210823_pB_wv02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
+      <c r="C53" s="4">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53" s="3">
+        <v>44431</v>
+      </c>
+      <c r="I53" t="s">
+        <v>141</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr11_20210823_pB_wv02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" s="4">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>13</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+      <c r="H54" s="3">
+        <v>44431</v>
+      </c>
+      <c r="I54" t="s">
+        <v>142</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr13_20210823_pB_wv03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1</v>
+      </c>
+      <c r="C55" s="4">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>14</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55" s="3">
+        <v>44431</v>
+      </c>
+      <c r="I55" t="s">
+        <v>143</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr14_20210823_pB_wv04</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L50" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
+  <autoFilter ref="A1:L55" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4557,10 +4734,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,7 +4811,7 @@
         <v>65</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J24" si="0">A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
+        <f t="shared" ref="J2:J33" si="0">A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
         <v>hr_sr01_20210430_pA_wv01</v>
       </c>
     </row>
@@ -5298,8 +5475,278 @@
         <v>hu_sr04_20210728_pA_wv03</v>
       </c>
     </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I25" t="s">
+        <v>144</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>hu_sr05_20210817_pA_wv04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>hu_sr06_20210824_pA_wv05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I27" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>hr_sr07_20210817_pA_wv06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ee_sr07_20210817_pA_wv06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sk_sr07_20210817_pA_wv06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I30" t="s">
+        <v>147</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>hr_sr08_20210824_pA_wv07</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="H31" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ee_sr08_20210824_pA_wv07</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32">
+        <v>7</v>
+      </c>
+      <c r="H32" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>sk_sr08_20210824_pA_wv07</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I33" t="s">
+        <v>146</v>
+      </c>
+      <c r="J33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>mt_sr02_20210817_pA_wv02</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L24" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}"/>
+  <autoFilter ref="A1:L33" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ipsos added new vars and new MT data
</commit_message>
<xml_diff>
--- a/data/spss_files_eu.xlsx
+++ b/data/spss_files_eu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8562358B-0BC0-4715-BAD8-647CFE6BA2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8394F87B-7721-4E14-84F8-27D012C3C997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="G2" sheetId="8" r:id="rId3"/>
     <sheet name="G3" sheetId="9" r:id="rId4"/>
     <sheet name="G2_archive" sheetId="10" r:id="rId5"/>
+    <sheet name="G3_archive" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'G2'!$A$1:$L$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">G2_archive!$A$1:$M$22</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'G3'!$A$1:$L$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'G3'!$A$1:$L$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="232">
   <si>
     <t>country</t>
   </si>
@@ -555,7 +556,190 @@
     <t>20-030971-01-17 LSHTM_MergedGroup2_Wave13_Final_v1_06102021_ICUO</t>
   </si>
   <si>
-    <t>20-030971_01_LSHTM_MT_Parent_Wave1_Final_v1_19102021_ICUO</t>
+    <t>20-030971_G3_Parents_MT_Wave1_v2_29112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Parents_MT_Wave2_v1_29112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave8_(1st additional)_FI&amp;LI_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave9_(2nd additional)_FI&amp;LI_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave10_(3rd additional)_FI&amp;LI_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave11_(4th additional)_FI&amp;LI_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave12_(5th additional)_FI&amp;LI_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave13_(6th additional)_FI&amp;LI_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave8_CH_v3_27102021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave9_CH_v3_27102021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave10_CH_v3_27102021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave11_CH_v3_27102021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave12_CH_v3_27102021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave13_CH_v3_27102021_IntClientUse</t>
+  </si>
+  <si>
+    <t>hr_sr01_20210430_pA_wv01</t>
+  </si>
+  <si>
+    <t>ee_sr01_20210430_pA_wv01</t>
+  </si>
+  <si>
+    <t>sk_sr01_20210430_pA_wv01</t>
+  </si>
+  <si>
+    <t>hr_sr02_20210521_pA_wv02</t>
+  </si>
+  <si>
+    <t>ee_sr02_20210521_pA_wv02</t>
+  </si>
+  <si>
+    <t>sk_sr02_20210521_pA_wv02</t>
+  </si>
+  <si>
+    <t>hr_sr04_20210611_pA_wv03</t>
+  </si>
+  <si>
+    <t>ee_sr04_20210611_pA_wv03</t>
+  </si>
+  <si>
+    <t>sk_sr04_20210611_pA_wv03</t>
+  </si>
+  <si>
+    <t>hr_sr05_20210713_pA_wv04</t>
+  </si>
+  <si>
+    <t>ee_sr05_20210713_pA_wv04</t>
+  </si>
+  <si>
+    <t>sk_sr05_20210713_pA_wv04</t>
+  </si>
+  <si>
+    <t>sk_sr06_20210728_pA_wv05</t>
+  </si>
+  <si>
+    <t>ee_sr06_20210728_pA_wv05</t>
+  </si>
+  <si>
+    <t>hr_sr06_20210728_pA_wv05</t>
+  </si>
+  <si>
+    <t>hr_sr07_20210817_pA_wv06</t>
+  </si>
+  <si>
+    <t>ee_sr07_20210817_pA_wv06</t>
+  </si>
+  <si>
+    <t>sk_sr07_20210817_pA_wv06</t>
+  </si>
+  <si>
+    <t>hr_sr08_20210824_pA_wv07</t>
+  </si>
+  <si>
+    <t>ee_sr08_20210824_pA_wv07</t>
+  </si>
+  <si>
+    <t>sk_sr08_20210824_pA_wv07</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave1_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave2_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave3_v2_11062021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave4_v2_09072021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave5_v2_28072021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave6_v2_06082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_Merged_HR EE SK_Wave7_v2_19082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>hu_sr01_20210611_pA_wv01</t>
+  </si>
+  <si>
+    <t>hu_sr03_20210716_pA_wv02</t>
+  </si>
+  <si>
+    <t>hu_sr04_20210728_pA_wv03</t>
+  </si>
+  <si>
+    <t>hu_sr05_20210817_pA_wv04</t>
+  </si>
+  <si>
+    <t>hu_sr06_20210824_pA_wv05</t>
+  </si>
+  <si>
+    <t>hu_sr08_20210916_pA_wv06</t>
+  </si>
+  <si>
+    <t>hu_sr09_20210927_pA_wv07</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave1_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave2_v2_14072021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave3_v2_28072021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave4_v2_03082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave5_v2_19082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave6_v2_19082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_HU_Wave7_v2_19082021_IntClientUse</t>
+  </si>
+  <si>
+    <t>mt_sr01_20210611_pA_wv01</t>
+  </si>
+  <si>
+    <t>mt_sr02_20210817_pA_wv02</t>
+  </si>
+  <si>
+    <t>mt_sr03_20210927_pA_wv03</t>
+  </si>
+  <si>
+    <t>20-030971_G3_MT_Wave1_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_MT_Wave2_v2_01112021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G3_MT_Wave3_v2_01112021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -618,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -627,6 +811,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,14 +1102,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -928,7 +1117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -936,7 +1125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -944,7 +1133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -952,7 +1141,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -960,7 +1149,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -982,16 +1171,16 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.87890625" style="2"/>
-    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.29296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1068,7 +1257,7 @@
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1290,7 @@
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1134,7 +1323,7 @@
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1167,7 +1356,7 @@
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1200,7 +1389,7 @@
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1233,7 +1422,7 @@
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1266,7 +1455,7 @@
         <v>pt_sr01_20210111_pA_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1299,7 +1488,7 @@
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1332,7 +1521,7 @@
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1365,7 +1554,7 @@
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1398,7 +1587,7 @@
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1431,7 +1620,7 @@
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +1653,7 @@
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1686,7 @@
         <v>pt_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1719,7 @@
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1563,7 +1752,7 @@
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1596,7 +1785,7 @@
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1629,7 +1818,7 @@
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1662,7 +1851,7 @@
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1695,7 +1884,7 @@
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1728,7 +1917,7 @@
         <v>pt_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -1761,7 +1950,7 @@
         <v>at_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1794,7 +1983,7 @@
         <v>dk_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1827,7 +2016,7 @@
         <v>fr_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
@@ -1860,7 +2049,7 @@
         <v>it_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
@@ -1893,7 +2082,7 @@
         <v>pl_sr04_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1926,7 +2115,7 @@
         <v>at_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1959,7 +2148,7 @@
         <v>dk_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1992,7 +2181,7 @@
         <v>fr_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -2025,7 +2214,7 @@
         <v>it_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
@@ -2058,7 +2247,7 @@
         <v>pl_sr05_20210226_pA_wv04</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -2130,7 +2319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -2160,7 +2349,7 @@
         <v>at_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>20</v>
       </c>
@@ -2191,7 +2380,7 @@
         <v>dk_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>22</v>
       </c>
@@ -2222,7 +2411,7 @@
         <v>fr_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
@@ -2253,7 +2442,7 @@
         <v>it_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
@@ -2284,7 +2473,7 @@
         <v>pl_sr06_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -2315,7 +2504,7 @@
         <v>es_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
@@ -2346,7 +2535,7 @@
         <v>pt_sr05_20210316_pA_wv05</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2376,7 +2565,7 @@
         <v>at_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2406,7 +2595,7 @@
         <v>dk_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -2436,7 +2625,7 @@
         <v>fr_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2466,7 +2655,7 @@
         <v>it_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2496,7 +2685,7 @@
         <v>pl_sr07_20210430_pA_wv06</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -2529,7 +2718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -2562,7 +2751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>21</v>
       </c>
@@ -2595,7 +2784,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -2628,7 +2817,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -2658,7 +2847,7 @@
         <v>at_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
@@ -2688,7 +2877,7 @@
         <v>dk_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>22</v>
       </c>
@@ -2718,7 +2907,7 @@
         <v>fr_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2748,7 +2937,7 @@
         <v>it_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -2778,7 +2967,7 @@
         <v>pl_sr08_20210413_pC_wv02</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>19</v>
       </c>
@@ -2808,7 +2997,7 @@
         <v>at_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>20</v>
       </c>
@@ -2838,7 +3027,7 @@
         <v>dk_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
@@ -2868,7 +3057,7 @@
         <v>fr_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -2898,7 +3087,7 @@
         <v>it_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>24</v>
       </c>
@@ -2928,7 +3117,7 @@
         <v>pl_sr09_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
@@ -2958,7 +3147,7 @@
         <v>es_sr08_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -2988,7 +3177,7 @@
         <v>pt_sr08_20210430_pA_wv07</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>21</v>
       </c>
@@ -3018,7 +3207,7 @@
         <v>es_sr09_20210521_pC_wv02</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>25</v>
       </c>
@@ -3058,27 +3247,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.41015625" customWidth="1"/>
-    <col min="2" max="2" width="10.41015625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.703125" customWidth="1"/>
-    <col min="4" max="4" width="8.703125" customWidth="1"/>
-    <col min="5" max="5" width="12.1171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.41015625" customWidth="1"/>
-    <col min="7" max="7" width="9.29296875" customWidth="1"/>
-    <col min="8" max="8" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="71.1171875" customWidth="1"/>
-    <col min="10" max="10" width="26.1171875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3116,7 +3305,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -3149,7 +3338,7 @@
         <v>fi_sr02_20210112_pC_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -3182,7 +3371,7 @@
         <v>ch_sr02_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -3218,7 +3407,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
@@ -3251,7 +3440,7 @@
         <v>lt_sr02_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3287,7 +3476,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -3321,7 +3510,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -3354,7 +3543,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3387,7 +3576,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -3417,7 +3606,7 @@
         <v>fi_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -3447,7 +3636,7 @@
         <v>lt_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3477,7 +3666,7 @@
         <v>ch_sr06_20210415_pC_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3508,7 +3697,7 @@
       </c>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>54</v>
       </c>
@@ -3541,7 +3730,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3574,7 +3763,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -3607,7 +3796,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -3640,7 +3829,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3670,7 +3859,7 @@
         <v>si_sr05_20210519_pA_wv04</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -3700,7 +3889,7 @@
         <v>gr_sr07_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -3730,7 +3919,7 @@
         <v>si_sr06_20210519_pA_wv05</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -3760,7 +3949,7 @@
         <v>gr_sr08_20210525_pA_wv06</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -3790,7 +3979,7 @@
         <v>si_sr07_20210525_pA_wv06</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -3820,7 +4009,7 @@
         <v>si_sr08_20210622_pA_wv07</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -3850,7 +4039,7 @@
         <v>gr_sr09_20210622_pA_wv07</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3860,27 +4049,27 @@
       <c r="C25" s="4">
         <v>4</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="10">
         <v>10</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25" s="3">
+      <c r="G25" s="10">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11">
         <v>44467</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>163</v>
+      <c r="I25" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr10_20210928_pB_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -3893,19 +4082,19 @@
       <c r="D26" s="2">
         <v>0</v>
       </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-      <c r="H26" s="3">
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="10">
+        <v>1</v>
+      </c>
+      <c r="H26" s="11">
         <v>44209</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="10" t="s">
         <v>34</v>
       </c>
       <c r="J26" s="2" t="str">
@@ -3916,7 +4105,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -3926,19 +4115,19 @@
       <c r="C27" s="4">
         <v>4</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="10">
         <v>3</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27">
+      <c r="F27" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="10">
         <v>2</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="11">
         <v>44376</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="10" t="s">
         <v>113</v>
       </c>
       <c r="J27" s="2" t="str">
@@ -3946,7 +4135,7 @@
         <v>ch_sr03_20210629_pA_wv02</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -3956,19 +4145,19 @@
       <c r="C28" s="4">
         <v>4</v>
       </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28">
+      <c r="E28" s="10">
+        <v>4</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="10">
         <v>3</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="11">
         <v>44376</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="10" t="s">
         <v>114</v>
       </c>
       <c r="J28" s="2" t="str">
@@ -3976,7 +4165,7 @@
         <v>ch_sr04_20210629_pA_wv03</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
@@ -3986,19 +4175,19 @@
       <c r="C29" s="4">
         <v>4</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="10">
         <v>5</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29">
-        <v>4</v>
-      </c>
-      <c r="H29" s="3">
+      <c r="F29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="10">
+        <v>4</v>
+      </c>
+      <c r="H29" s="11">
         <v>44376</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="10" t="s">
         <v>115</v>
       </c>
       <c r="J29" s="2" t="str">
@@ -4006,7 +4195,7 @@
         <v>ch_sr05_20210629_pA_wv04</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -4016,19 +4205,19 @@
       <c r="C30" s="4">
         <v>4</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="10">
         <v>7</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30">
+      <c r="F30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="10">
         <v>5</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="11">
         <v>44376</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="10" t="s">
         <v>116</v>
       </c>
       <c r="J30" s="2" t="str">
@@ -4036,7 +4225,7 @@
         <v>ch_sr07_20210629_pA_wv05</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -4046,19 +4235,19 @@
       <c r="C31" s="4">
         <v>4</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="10">
         <v>8</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31">
+      <c r="F31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="10">
         <v>6</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="11">
         <v>44376</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="10" t="s">
         <v>117</v>
       </c>
       <c r="J31" s="2" t="str">
@@ -4066,7 +4255,7 @@
         <v>ch_sr08_20210629_pA_wv06</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -4076,19 +4265,19 @@
       <c r="C32" s="4">
         <v>4</v>
       </c>
-      <c r="E32">
-        <v>9</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32">
+      <c r="E32" s="10">
+        <v>9</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="10">
         <v>7</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="11">
         <v>44376</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="10" t="s">
         <v>118</v>
       </c>
       <c r="J32" s="2" t="str">
@@ -4096,7 +4285,7 @@
         <v>ch_sr09_20210629_pA_wv07</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -4132,7 +4321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -4162,7 +4351,7 @@
         <v>fi_sr03_20210629_pA_wv02</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -4192,7 +4381,7 @@
         <v>fi_sr04_20210629_pA_wv03</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -4222,7 +4411,7 @@
         <v>fi_sr05_20210629_pA_wv04</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -4252,7 +4441,7 @@
         <v>fi_sr07_20210629_pA_wv05</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -4282,7 +4471,7 @@
         <v>fi_sr08_20210629_pA_wv06</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
@@ -4312,7 +4501,7 @@
         <v>fi_sr09_20210629_pA_wv07</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -4348,7 +4537,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
@@ -4378,7 +4567,7 @@
         <v>lt_sr03_20210629_pA_wv02</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>35</v>
       </c>
@@ -4408,7 +4597,7 @@
         <v>lt_sr04_20210629_pA_wv03</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>35</v>
       </c>
@@ -4438,7 +4627,7 @@
         <v>lt_sr05_20210629_pA_wv04</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
@@ -4468,7 +4657,7 @@
         <v>lt_sr07_20210629_pA_wv05</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
@@ -4478,19 +4667,19 @@
       <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="10">
         <v>8</v>
       </c>
-      <c r="F45" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45">
+      <c r="F45" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="10">
         <v>6</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="11">
         <v>44376</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="I45" s="10" t="s">
         <v>128</v>
       </c>
       <c r="J45" s="2" t="str">
@@ -4498,7 +4687,7 @@
         <v>lt_sr08_20210629_pA_wv06</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>35</v>
       </c>
@@ -4508,19 +4697,19 @@
       <c r="C46" s="2">
         <v>4</v>
       </c>
-      <c r="E46">
-        <v>9</v>
-      </c>
-      <c r="F46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46">
+      <c r="E46" s="10">
+        <v>9</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="10">
         <v>7</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="11">
         <v>44376</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" s="10" t="s">
         <v>129</v>
       </c>
       <c r="J46" s="2" t="str">
@@ -4528,7 +4717,7 @@
         <v>lt_sr09_20210629_pA_wv07</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -4558,7 +4747,7 @@
         <v>fi_sr10_20210723_pB_wv01</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -4568,27 +4757,27 @@
       <c r="C48">
         <v>4</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="10">
         <v>10</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" s="3">
-        <v>44400</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>134</v>
+      <c r="G48" s="10">
+        <v>1</v>
+      </c>
+      <c r="H48" s="11">
+        <v>44501</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr10_20210723_pB_wv01</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
+        <v>lt_sr10_20211101_pB_wv01</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -4598,19 +4787,19 @@
       <c r="C49">
         <v>4</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="10">
         <v>11</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49" s="3">
+      <c r="G49" s="10">
+        <v>1</v>
+      </c>
+      <c r="H49" s="11">
         <v>44400</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="10" t="s">
         <v>135</v>
       </c>
       <c r="J49" t="str">
@@ -4618,7 +4807,7 @@
         <v>ch_sr11_20210723_pD_wv01</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -4628,27 +4817,27 @@
       <c r="C50">
         <v>4</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="10">
         <v>12</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="10">
         <v>2</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="11">
         <v>44467</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>164</v>
+      <c r="I50" s="10" t="s">
+        <v>179</v>
       </c>
       <c r="J50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr12_20210928_pB_wv02</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -4678,7 +4867,7 @@
         <v>si_sr09_20210716_pC_wv02</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -4708,7 +4897,7 @@
         <v>fi_sr11_20210823_pB_wv02</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -4718,27 +4907,27 @@
       <c r="C53" s="4">
         <v>4</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="10">
         <v>11</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="10">
         <v>2</v>
       </c>
-      <c r="H53" s="3">
-        <v>44431</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>141</v>
+      <c r="H53" s="11">
+        <v>44501</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>173</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr11_20210823_pB_wv02</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
+        <v>lt_sr11_20211101_pB_wv02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -4748,27 +4937,27 @@
       <c r="C54" s="4">
         <v>4</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="10">
         <v>13</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="10">
         <v>3</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="11">
         <v>44467</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>165</v>
+      <c r="I54" s="10" t="s">
+        <v>180</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr13_20210928_pB_wv03</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>37</v>
       </c>
@@ -4778,27 +4967,27 @@
       <c r="C55" s="4">
         <v>4</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="10">
         <v>14</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G55">
-        <v>4</v>
-      </c>
-      <c r="H55" s="3">
+      <c r="G55" s="10">
+        <v>4</v>
+      </c>
+      <c r="H55" s="11">
         <v>44467</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>166</v>
+      <c r="I55" s="10" t="s">
+        <v>181</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr14_20210928_pB_wv04</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -4828,7 +5017,7 @@
         <v>fi_sr12_20210916_pB_wv03</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -4838,27 +5027,27 @@
       <c r="C57" s="4">
         <v>4</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="10">
         <v>12</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="10">
         <v>3</v>
       </c>
-      <c r="H57" s="3">
-        <v>44455</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>152</v>
+      <c r="H57" s="11">
+        <v>44501</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>174</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr12_20210916_pB_wv03</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
+        <v>lt_sr12_20211101_pB_wv03</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -4868,27 +5057,27 @@
       <c r="C58" s="4">
         <v>4</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="10">
         <v>15</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="10">
         <v>5</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H58" s="11">
         <v>44467</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>167</v>
+      <c r="I58" s="10" t="s">
+        <v>182</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr15_20210928_pB_wv05</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -4898,27 +5087,27 @@
       <c r="C59" s="4">
         <v>4</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="10">
         <v>16</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="10">
         <v>6</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59" s="11">
         <v>44466</v>
       </c>
-      <c r="I59" t="s">
-        <v>154</v>
+      <c r="I59" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
         <v>ch_sr16_20210927_pB_wv06</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>35</v>
       </c>
@@ -4928,27 +5117,27 @@
       <c r="C60">
         <v>4</v>
       </c>
-      <c r="E60">
-        <v>14</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E60" s="10">
+        <v>13</v>
+      </c>
+      <c r="F60" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G60">
-        <v>5</v>
-      </c>
-      <c r="H60" s="3">
-        <v>44466</v>
-      </c>
-      <c r="I60" t="s">
-        <v>155</v>
+      <c r="G60" s="10">
+        <v>4</v>
+      </c>
+      <c r="H60" s="11">
+        <v>44501</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr14_20210927_pB_wv05</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.5">
+        <v>lt_sr13_20211101_pB_wv04</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -4978,7 +5167,7 @@
         <v>fi_sr14_20210927_pB_wv05</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -5008,7 +5197,7 @@
         <v>fi_sr13_20210928_pB_wv04</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>35</v>
       </c>
@@ -5018,27 +5207,27 @@
       <c r="C63">
         <v>4</v>
       </c>
-      <c r="E63">
-        <v>13</v>
-      </c>
-      <c r="F63" s="4" t="s">
+      <c r="E63" s="10">
+        <v>14</v>
+      </c>
+      <c r="F63" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G63">
-        <v>4</v>
-      </c>
-      <c r="H63" s="3">
-        <v>44467</v>
-      </c>
-      <c r="I63" t="s">
-        <v>168</v>
+      <c r="G63" s="10">
+        <v>5</v>
+      </c>
+      <c r="H63" s="11">
+        <v>44501</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr13_20210928_pB_wv04</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.5">
+        <v>lt_sr14_20211101_pB_wv05</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -5068,7 +5257,7 @@
         <v>fi_sr15_20211007_pB_wv06</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>35</v>
       </c>
@@ -5078,28 +5267,28 @@
       <c r="C65">
         <v>4</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="10">
         <v>15</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="10">
         <v>6</v>
       </c>
-      <c r="H65" s="3">
-        <v>44476</v>
-      </c>
-      <c r="I65" t="s">
-        <v>169</v>
+      <c r="H65" s="11">
+        <v>44501</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>177</v>
       </c>
       <c r="J65" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr15_20211007_pB_wv06</v>
+        <v>lt_sr15_20211101_pB_wv06</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L63" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
+  <autoFilter ref="A1:L65" xr:uid="{F3EFC057-A940-A84A-81E0-6D8DDFAC2A47}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5107,20 +5296,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="62" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5158,7 +5347,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -5178,17 +5367,17 @@
         <v>1</v>
       </c>
       <c r="H2" s="3">
-        <v>44316</v>
+        <v>44501</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J41" si="0">A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
-        <v>hr_sr01_20210430_pA_wv01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+        <f t="shared" ref="J2:J42" si="0">A2&amp;"_"&amp;"sr"&amp;TEXT(E2,"00")&amp;"_"&amp;YEAR(H2)&amp;TEXT(H2,"MM")&amp;TEXT(H2,"DD")&amp;"_p"&amp;F2&amp;"_wv"&amp;TEXT(G2,"00")&amp;""</f>
+        <v>hr_sr01_20211101_pA_wv01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -5208,17 +5397,17 @@
         <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>44316</v>
+        <v>44501</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="J3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr01_20210430_pA_wv01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+        <v>ee_sr01_20211101_pA_wv01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -5238,17 +5427,17 @@
         <v>1</v>
       </c>
       <c r="H4" s="3">
-        <v>44316</v>
+        <v>44501</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr01_20210430_pA_wv01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+        <v>sk_sr01_20211101_pA_wv01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -5268,17 +5457,17 @@
         <v>2</v>
       </c>
       <c r="H5" s="3">
-        <v>44337</v>
-      </c>
-      <c r="I5" t="s">
-        <v>79</v>
+        <v>44501</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>hr_sr02_20210521_pA_wv02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+        <v>hr_sr02_20211101_pA_wv02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
@@ -5298,17 +5487,17 @@
         <v>2</v>
       </c>
       <c r="H6" s="3">
-        <v>44337</v>
-      </c>
-      <c r="I6" t="s">
-        <v>79</v>
+        <v>44501</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr02_20210521_pA_wv02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+        <v>ee_sr02_20211101_pA_wv02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
@@ -5328,17 +5517,17 @@
         <v>2</v>
       </c>
       <c r="H7" s="3">
-        <v>44337</v>
-      </c>
-      <c r="I7" t="s">
-        <v>79</v>
+        <v>44501</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr02_20210521_pA_wv02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+        <v>sk_sr02_20211101_pA_wv02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -5368,7 +5557,7 @@
         <v>hr_sr03_20210622_pC_wv01</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -5398,7 +5587,7 @@
         <v>ee_sr03_20210622_pC_wv01</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -5428,7 +5617,7 @@
         <v>sk_sr03_20210622_pC_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -5448,17 +5637,17 @@
         <v>1</v>
       </c>
       <c r="H11" s="3">
-        <v>44358</v>
+        <v>44501</v>
       </c>
       <c r="I11" t="s">
-        <v>109</v>
+        <v>229</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>mt_sr01_20210611_pA_wv01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+        <v>mt_sr01_20211101_pA_wv01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -5481,14 +5670,14 @@
         <v>44358</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>219</v>
       </c>
       <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr01_20210611_pA_wv01</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -5518,7 +5707,7 @@
         <v>hu_sr02_20210623_pC_wv01</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -5538,17 +5727,17 @@
         <v>3</v>
       </c>
       <c r="H14" s="3">
-        <v>44358</v>
+        <v>44501</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>hr_sr04_20210611_pA_wv03</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+        <v>hr_sr04_20211101_pA_wv03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -5568,17 +5757,17 @@
         <v>3</v>
       </c>
       <c r="H15" s="3">
-        <v>44358</v>
+        <v>44501</v>
       </c>
       <c r="I15" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr04_20210611_pA_wv03</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+        <v>ee_sr04_20211101_pA_wv03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -5598,17 +5787,17 @@
         <v>3</v>
       </c>
       <c r="H16" s="3">
-        <v>44358</v>
+        <v>44501</v>
       </c>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>207</v>
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr04_20210611_pA_wv03</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+        <v>sk_sr04_20211101_pA_wv03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -5628,17 +5817,17 @@
         <v>4</v>
       </c>
       <c r="H17" s="3">
-        <v>44390</v>
+        <v>44501</v>
       </c>
       <c r="I17" t="s">
-        <v>132</v>
+        <v>208</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>hr_sr05_20210713_pA_wv04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+        <v>hr_sr05_20211101_pA_wv04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -5658,17 +5847,17 @@
         <v>4</v>
       </c>
       <c r="H18" s="3">
-        <v>44390</v>
+        <v>44501</v>
       </c>
       <c r="I18" t="s">
-        <v>132</v>
+        <v>208</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr05_20210713_pA_wv04</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+        <v>ee_sr05_20211101_pA_wv04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -5688,17 +5877,17 @@
         <v>4</v>
       </c>
       <c r="H19" s="3">
-        <v>44390</v>
+        <v>44501</v>
       </c>
       <c r="I19" t="s">
-        <v>132</v>
+        <v>208</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr05_20210713_pA_wv04</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+        <v>sk_sr05_20211101_pA_wv04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -5721,14 +5910,14 @@
         <v>44393</v>
       </c>
       <c r="I20" t="s">
-        <v>133</v>
+        <v>220</v>
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr03_20210716_pA_wv02</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -5748,17 +5937,17 @@
         <v>5</v>
       </c>
       <c r="H21" s="3">
-        <v>44405</v>
+        <v>44501</v>
       </c>
       <c r="I21" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr06_20210728_pA_wv05</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+        <v>sk_sr06_20211101_pA_wv05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -5778,17 +5967,17 @@
         <v>5</v>
       </c>
       <c r="H22" s="3">
-        <v>44405</v>
+        <v>44501</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr06_20210728_pA_wv05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+        <v>ee_sr06_20211101_pA_wv05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -5808,17 +5997,17 @@
         <v>5</v>
       </c>
       <c r="H23" s="3">
-        <v>44405</v>
+        <v>44501</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>hr_sr06_20210728_pA_wv05</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+        <v>hr_sr06_20211101_pA_wv05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -5841,14 +6030,14 @@
         <v>44405</v>
       </c>
       <c r="I24" t="s">
-        <v>139</v>
+        <v>221</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr04_20210728_pA_wv03</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -5871,14 +6060,14 @@
         <v>44425</v>
       </c>
       <c r="I25" t="s">
-        <v>144</v>
+        <v>222</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr05_20210817_pA_wv04</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -5901,14 +6090,14 @@
         <v>44432</v>
       </c>
       <c r="I26" t="s">
-        <v>148</v>
+        <v>223</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr06_20210824_pA_wv05</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -5928,17 +6117,17 @@
         <v>6</v>
       </c>
       <c r="H27" s="3">
-        <v>44425</v>
+        <v>44501</v>
       </c>
       <c r="I27" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>hr_sr07_20210817_pA_wv06</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+        <v>hr_sr07_20211101_pA_wv06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -5958,17 +6147,17 @@
         <v>6</v>
       </c>
       <c r="H28" s="3">
-        <v>44425</v>
+        <v>44501</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr07_20210817_pA_wv06</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
+        <v>ee_sr07_20211101_pA_wv06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -5988,17 +6177,17 @@
         <v>6</v>
       </c>
       <c r="H29" s="3">
-        <v>44425</v>
+        <v>44501</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>145</v>
+        <v>210</v>
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr07_20210817_pA_wv06</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
+        <v>sk_sr07_20211101_pA_wv06</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -6018,17 +6207,17 @@
         <v>7</v>
       </c>
       <c r="H30" s="3">
-        <v>44432</v>
+        <v>44501</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
       <c r="J30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>hr_sr08_20210824_pA_wv07</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.5">
+        <v>hr_sr08_20211101_pA_wv07</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>67</v>
       </c>
@@ -6048,17 +6237,17 @@
         <v>7</v>
       </c>
       <c r="H31" s="3">
-        <v>44432</v>
+        <v>44501</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
       <c r="J31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ee_sr08_20210824_pA_wv07</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.5">
+        <v>ee_sr08_20211101_pA_wv07</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
@@ -6078,17 +6267,17 @@
         <v>7</v>
       </c>
       <c r="H32" s="3">
-        <v>44432</v>
+        <v>44501</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
       <c r="J32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sk_sr08_20210824_pA_wv07</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.5">
+        <v>sk_sr08_20211101_pA_wv07</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>111</v>
       </c>
@@ -6108,17 +6297,17 @@
         <v>2</v>
       </c>
       <c r="H33" s="3">
-        <v>44425</v>
+        <v>44501</v>
       </c>
       <c r="I33" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
       <c r="J33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>mt_sr02_20210817_pA_wv02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.5">
+        <v>mt_sr02_20211101_pA_wv02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -6148,7 +6337,7 @@
         <v>hu_sr07_20210916_pC_wv02</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -6170,15 +6359,15 @@
       <c r="H35" s="3">
         <v>44455</v>
       </c>
-      <c r="I35" t="s">
-        <v>150</v>
+      <c r="I35" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr08_20210916_pA_wv06</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
@@ -6208,7 +6397,7 @@
         <v>hr_sr09_20210916_pC_wv02</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
@@ -6238,7 +6427,7 @@
         <v>ee_sr09_20210916_pC_wv02</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -6268,7 +6457,7 @@
         <v>sk_sr09_20210916_pC_wv02</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>83</v>
       </c>
@@ -6290,15 +6479,15 @@
       <c r="H39" s="3">
         <v>44466</v>
       </c>
-      <c r="I39" t="s">
-        <v>156</v>
+      <c r="I39" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
         <v>hu_sr09_20210927_pA_wv07</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>111</v>
       </c>
@@ -6318,17 +6507,17 @@
         <v>3</v>
       </c>
       <c r="H40" s="3">
-        <v>44466</v>
+        <v>44501</v>
       </c>
       <c r="I40" t="s">
-        <v>157</v>
+        <v>231</v>
       </c>
       <c r="J40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>mt_sr03_20210927_pA_wv03</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.5">
+        <v>mt_sr03_20211101_pA_wv03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>111</v>
       </c>
@@ -6348,46 +6537,76 @@
         <v>1</v>
       </c>
       <c r="H41" s="3">
-        <v>44489</v>
+        <v>44529</v>
       </c>
       <c r="I41" t="s">
         <v>170</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>mt_sr04_20211020_pC_wv01</v>
+        <v>mt_sr04_20211129_pC_wv01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>44529</v>
+      </c>
+      <c r="I42" t="s">
+        <v>171</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v>mt_sr05_20211129_pC_wv02</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L40" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}"/>
+  <autoFilter ref="A1:L42" xr:uid="{351EBC7F-6B8C-4AA7-9B22-1E80FDAC23FE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED305700-03AC-46AC-97A8-F43280C410DF}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24:J27"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.87890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.87890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.87890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.41015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6428,7 +6647,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -6463,7 +6682,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -6498,7 +6717,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -6530,7 +6749,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>37</v>
       </c>
@@ -6562,7 +6781,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -6594,7 +6813,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -6626,7 +6845,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -6658,7 +6877,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -6693,7 +6912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -6728,7 +6947,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -6760,7 +6979,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -6792,7 +7011,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -6824,7 +7043,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -6856,7 +7075,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -6888,7 +7107,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -6923,7 +7142,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -6958,7 +7177,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -6990,7 +7209,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -7022,7 +7241,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -7054,7 +7273,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -7086,7 +7305,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
@@ -7118,7 +7337,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -7144,7 +7363,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
@@ -7170,7 +7389,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -7196,7 +7415,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -7222,7 +7441,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -7246,10 +7465,1230 @@
       </c>
       <c r="J27" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="7">
+        <v>10</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="7">
+        <v>1</v>
+      </c>
+      <c r="H28" s="8">
+        <v>44400</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="7">
+        <v>11</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" s="7">
+        <v>2</v>
+      </c>
+      <c r="H29" s="8">
+        <v>44431</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="7">
+        <v>12</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="7">
+        <v>3</v>
+      </c>
+      <c r="H30" s="8">
+        <v>44455</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="7">
+        <v>14</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="7">
+        <v>5</v>
+      </c>
+      <c r="H31" s="8">
+        <v>44466</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="7">
+        <v>13</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="7">
+        <v>4</v>
+      </c>
+      <c r="H32" s="8">
+        <v>44467</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="7">
+        <v>15</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="7">
+        <v>6</v>
+      </c>
+      <c r="H33" s="8">
+        <v>44476</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="7">
+        <v>10</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="7">
+        <v>1</v>
+      </c>
+      <c r="H34" s="8">
+        <v>44467</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="7">
+        <v>12</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" s="7">
+        <v>2</v>
+      </c>
+      <c r="H35" s="8">
+        <v>44467</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="7">
+        <v>13</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="7">
+        <v>3</v>
+      </c>
+      <c r="H36" s="8">
+        <v>44467</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="7">
+        <v>14</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="7">
+        <v>4</v>
+      </c>
+      <c r="H37" s="8">
+        <v>44467</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="7">
+        <v>15</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G38" s="7">
+        <v>5</v>
+      </c>
+      <c r="H38" s="8">
+        <v>44467</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="7">
+        <v>16</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39" s="7">
+        <v>6</v>
+      </c>
+      <c r="H39" s="8">
+        <v>44466</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M22" xr:uid="{ED305700-03AC-46AC-97A8-F43280C410DF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1C614B-B97D-4698-ACE6-E0CD780C08D7}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>44316</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>44337</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>44358</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
+        <v>44358</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
+        <v>44358</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>44390</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>44390</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3">
+        <v>44390</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>44405</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>44405</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3">
+        <v>44405</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6</v>
+      </c>
+      <c r="H18" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="2">
+        <v>6</v>
+      </c>
+      <c r="H19" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2">
+        <v>8</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="2">
+        <v>7</v>
+      </c>
+      <c r="H20" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2">
+        <v>8</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7</v>
+      </c>
+      <c r="H21" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2">
+        <v>7</v>
+      </c>
+      <c r="H22" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>44358</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3">
+        <v>44393</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3">
+        <v>44405</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2">
+        <v>5</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
+        <v>6</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2">
+        <v>5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>44432</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="2">
+        <v>6</v>
+      </c>
+      <c r="H28" s="3">
+        <v>44455</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>9</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="2">
+        <v>7</v>
+      </c>
+      <c r="H29" s="3">
+        <v>44466</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>44358</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>44425</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3</v>
+      </c>
+      <c r="H32" s="3">
+        <v>44466</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>